<commit_message>
Versão finalizada com cadastro de cid, alteração de status e relatórios.
</commit_message>
<xml_diff>
--- a/script_base_dados/grants.xlsx
+++ b/script_base_dados/grants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\integracao\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47119A9B-87FC-4E9D-8207-A29BE869512B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4A4D1B-ECC6-49A0-A0D0-D54A93955E25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="82">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -278,57 +278,6 @@
   </si>
   <si>
     <t>PASSWORD '1234';</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to mmattos;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to mmattos;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to mmattos;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to mmattos;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to mmattos;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to mmattos;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to mmattos;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to mmattos;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to mmattos;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO mmattos;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO mmattos;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  mmattos;</t>
-  </si>
-  <si>
-    <t>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO mmattos;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO mmattos;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO mmattos;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO mmattos;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO mmattos;</t>
   </si>
   <si>
     <t>Falta criar na aplicação e associar ao grupo de acesso</t>
@@ -3168,7 +3117,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3182,7 +3131,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3334,14 +3283,14 @@
         <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
         <v>80</v>
       </c>
       <c r="D22" t="str">
         <f>A22&amp;" "&amp;B22&amp;" "&amp;C22</f>
-        <v>CREATE USER  aoliveira PASSWORD '1234';</v>
+        <v>CREATE USER  ronan PASSWORD '1234';</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3349,14 +3298,14 @@
         <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
       </c>
       <c r="D23" t="str">
-        <f>A23&amp;" "&amp;B23&amp;C23</f>
-        <v>GRANT CONNECT ON DATABASE vilaverde_dw TO  aoliveira;</v>
+        <f t="shared" ref="D23:D83" si="0">A23&amp;" "&amp;B23&amp;" "&amp;C23</f>
+        <v>GRANT CONNECT ON DATABASE vilaverde_dw TO  ronan ;</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3364,14 +3313,14 @@
         <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" ref="D24:D35" si="0">A24&amp;" "&amp;B24&amp;C24</f>
-        <v>GRANT USAGE ON SCHEMA integracao TO  aoliveira;</v>
+        <f t="shared" si="0"/>
+        <v>GRANT USAGE ON SCHEMA integracao TO  ronan ;</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3379,14 +3328,14 @@
         <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  aoliveira;</v>
+        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  ronan ;</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3394,14 +3343,14 @@
         <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  aoliveira;</v>
+        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  ronan ;</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3409,14 +3358,14 @@
         <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO aoliveira;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO ronan ;</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3424,14 +3373,14 @@
         <v>71</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  aoliveira;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  ronan ;</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3439,14 +3388,14 @@
         <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  aoliveira;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  ronan ;</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3454,14 +3403,14 @@
         <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  aoliveira;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  ronan ;</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3469,14 +3418,14 @@
         <v>74</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  aoliveira;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  ronan ;</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3484,14 +3433,14 @@
         <v>75</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  aoliveira;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  ronan ;</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3499,14 +3448,14 @@
         <v>76</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  aoliveira;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  ronan ;</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3514,14 +3463,14 @@
         <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  aoliveira;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  ronan ;</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3529,14 +3478,14 @@
         <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  aoliveira;</v>
+        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  ronan ;</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3544,13 +3493,14 @@
         <v>27</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
       </c>
-      <c r="D36" t="s">
-        <v>81</v>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to ronan ;</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3558,13 +3508,14 @@
         <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
       </c>
-      <c r="D37" t="s">
-        <v>82</v>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to ronan ;</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3572,13 +3523,14 @@
         <v>26</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
         <v>1</v>
       </c>
-      <c r="D38" t="s">
-        <v>83</v>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to ronan ;</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3586,13 +3538,14 @@
         <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
       </c>
-      <c r="D39" t="s">
-        <v>84</v>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to ronan ;</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3600,13 +3553,14 @@
         <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
       </c>
-      <c r="D40" t="s">
-        <v>85</v>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to ronan ;</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3614,13 +3568,14 @@
         <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
       </c>
-      <c r="D41" t="s">
-        <v>86</v>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to ronan ;</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3628,13 +3583,14 @@
         <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
       </c>
-      <c r="D42" t="s">
-        <v>87</v>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to ronan ;</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3642,13 +3598,14 @@
         <v>23</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
       </c>
-      <c r="D43" t="s">
-        <v>88</v>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to ronan ;</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3656,13 +3613,14 @@
         <v>24</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C44" t="s">
         <v>1</v>
       </c>
-      <c r="D44" t="s">
-        <v>89</v>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to ronan ;</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3670,13 +3628,14 @@
         <v>0</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C45" t="s">
         <v>1</v>
       </c>
-      <c r="D45" t="s">
-        <v>90</v>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO ronan ;</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3684,13 +3643,14 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C46" t="s">
         <v>1</v>
       </c>
-      <c r="D46" t="s">
-        <v>91</v>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO ronan ;</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3698,13 +3658,14 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C47" t="s">
         <v>1</v>
       </c>
-      <c r="D47" t="s">
-        <v>92</v>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  ronan ;</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3712,13 +3673,14 @@
         <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
       </c>
-      <c r="D48" t="s">
-        <v>93</v>
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO ronan ;</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3726,13 +3688,14 @@
         <v>5</v>
       </c>
       <c r="B49" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C49" t="s">
         <v>1</v>
       </c>
-      <c r="D49" t="s">
-        <v>94</v>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO ronan ;</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3740,13 +3703,14 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
         <v>1</v>
       </c>
-      <c r="D50" t="s">
-        <v>95</v>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO ronan ;</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3754,13 +3718,14 @@
         <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C51" t="s">
         <v>1</v>
       </c>
-      <c r="D51" t="s">
-        <v>96</v>
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO ronan ;</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3768,13 +3733,194 @@
         <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C52" t="s">
         <v>1</v>
       </c>
-      <c r="D52" t="s">
-        <v>97</v>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO ronan ;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D62" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D63" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D64" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D73" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D74" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D75" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D76" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D77" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D78" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D79" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D80" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Entrega do Gestão de Leitos Web e relatórios em PDF
</commit_message>
<xml_diff>
--- a/script_base_dados/grants.xlsx
+++ b/script_base_dados/grants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\integracao\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4A4D1B-ECC6-49A0-A0D0-D54A93955E25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9523E7D9-F316-40BE-AD7F-3A052CD815D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="95">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -235,9 +235,6 @@
     <t>ronan</t>
   </si>
   <si>
-    <t xml:space="preserve">GRANT CONNECT ON DATABASE vilaverde_dw TO </t>
-  </si>
-  <si>
     <t xml:space="preserve">GRANT USAGE ON SCHEMA integracao TO </t>
   </si>
   <si>
@@ -281,6 +278,48 @@
   </si>
   <si>
     <t>Falta criar na aplicação e associar ao grupo de acesso</t>
+  </si>
+  <si>
+    <t>camila</t>
+  </si>
+  <si>
+    <t>adminstrativo</t>
+  </si>
+  <si>
+    <t>tivilaverde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT SELECT on integracao.tb_leito TO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT SELECT on integracao.vw_ctrl_leito TO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT SELECT on integracao.tb_mtvo_alta TO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT CONNECT ON DATABASE vila_verde TO </t>
+  </si>
+  <si>
+    <t>Gabriela Reis</t>
+  </si>
+  <si>
+    <t>Letícia Delgado</t>
+  </si>
+  <si>
+    <t>Daniella Eliza Mendes de Souza Santos</t>
+  </si>
+  <si>
+    <t>greis</t>
+  </si>
+  <si>
+    <t>ldelgado</t>
+  </si>
+  <si>
+    <t>deliza</t>
   </si>
 </sst>
 </file>
@@ -3117,13 +3156,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="97.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="95.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
@@ -3131,7 +3170,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3246,7 +3285,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
@@ -3254,7 +3293,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>60</v>
       </c>
@@ -3262,7 +3301,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
@@ -3270,7 +3309,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>64</v>
       </c>
@@ -3278,628 +3317,659 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>79</v>
-      </c>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" t="str">
-        <f>A22&amp;" "&amp;B22&amp;" "&amp;C22</f>
-        <v>CREATE USER  ronan PASSWORD '1234';</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>66</v>
-      </c>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" t="str">
-        <f t="shared" ref="D23:D83" si="0">A23&amp;" "&amp;B23&amp;" "&amp;C23</f>
-        <v>GRANT CONNECT ON DATABASE vilaverde_dw TO  ronan ;</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>67</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT USAGE ON SCHEMA integracao TO  ronan ;</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>68</v>
-      </c>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  ronan ;</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>69</v>
-      </c>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  ronan ;</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>70</v>
-      </c>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO ronan ;</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>71</v>
-      </c>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  ronan ;</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>72</v>
-      </c>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  ronan ;</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>73</v>
-      </c>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  ronan ;</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>74</v>
-      </c>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  ronan ;</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  ronan ;</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  ronan ;</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  ronan ;</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>78</v>
-      </c>
-      <c r="B35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  ronan ;</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>27</v>
-      </c>
-      <c r="B36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to ronan ;</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="B37" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C37" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="D37" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to ronan ;</v>
+        <f>A37&amp;" "&amp;B37&amp;" "&amp;C37</f>
+        <v>CREATE USER  deliza PASSWORD '1234';</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="B38" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C38" t="s">
         <v>1</v>
       </c>
       <c r="D38" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to ronan ;</v>
+        <f t="shared" ref="D38:D98" si="0">A38&amp;" "&amp;B38&amp;" "&amp;C38</f>
+        <v>GRANT CONNECT ON DATABASE vila_verde TO  deliza ;</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to ronan ;</v>
+        <v>GRANT USAGE ON SCHEMA integracao TO  deliza ;</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to ronan ;</v>
+        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  deliza ;</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to ronan ;</v>
+        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  deliza ;</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="B42" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to ronan ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO deliza ;</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="B43" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to ronan ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  deliza ;</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B44" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C44" t="s">
         <v>1</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to ronan ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  deliza ;</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="B45" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C45" t="s">
         <v>1</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO ronan ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  deliza ;</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="B46" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C46" t="s">
         <v>1</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO ronan ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  deliza ;</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C47" t="s">
         <v>1</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  ronan ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  deliza ;</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="B48" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO ronan ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  deliza ;</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="B49" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
         <v>1</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO ronan ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  deliza ;</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="B50" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C50" t="s">
         <v>1</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO ronan ;</v>
+        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  deliza ;</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B51" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C51" t="s">
         <v>1</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO ronan ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to deliza ;</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to deliza ;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to deliza ;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to deliza ;</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to deliza ;</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to deliza ;</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to deliza ;</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to deliza ;</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to deliza ;</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO deliza ;</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO deliza ;</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  deliza ;</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" t="s">
+        <v>94</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO deliza ;</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO deliza ;</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" t="s">
+        <v>94</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO deliza ;</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" t="s">
+        <v>94</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO deliza ;</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>8</v>
       </c>
-      <c r="B52" t="s">
-        <v>65</v>
-      </c>
-      <c r="C52" t="s">
-        <v>1</v>
-      </c>
-      <c r="D52" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO ronan ;</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D54" t="str">
+      <c r="B67" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO deliza ;</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>86</v>
+      </c>
+      <c r="B68" t="s">
+        <v>94</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  deliza ;</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>87</v>
+      </c>
+      <c r="B69" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  deliza ;</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>84</v>
+      </c>
+      <c r="B70" t="s">
+        <v>94</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.tb_leito TO  deliza ;</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>85</v>
+      </c>
+      <c r="B71" t="s">
+        <v>94</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  deliza ;</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D72" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  </v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D55" t="str">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D73" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  </v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D56" t="str">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D74" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  </v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D57" t="str">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D75" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  </v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D58" t="str">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D76" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  </v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D59" t="str">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D77" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  </v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D60" t="str">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D78" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  </v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D61" t="str">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D79" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  </v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D62" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D63" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D64" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D66" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D67" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D68" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D69" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D70" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D71" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D72" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D73" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D74" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D75" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D76" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D77" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D78" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D79" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D80" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  </v>
@@ -3923,7 +3993,98 @@
         <v xml:space="preserve">  </v>
       </c>
     </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D88" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D89" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D90" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D91" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D92" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D93" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D94" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D95" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D96" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D97" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D98" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Criação do Relatório por tipo
</commit_message>
<xml_diff>
--- a/script_base_dados/grants.xlsx
+++ b/script_base_dados/grants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\integracao\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9523E7D9-F316-40BE-AD7F-3A052CD815D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D752F44-E061-4D33-A660-FEB3EF95D2BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="111">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -320,6 +320,54 @@
   </si>
   <si>
     <t>deliza</t>
+  </si>
+  <si>
+    <t>Alaim Albino de Oliveira</t>
+  </si>
+  <si>
+    <t>Regiane Katia de Almeida Freitas</t>
+  </si>
+  <si>
+    <t>Beatriz Rocha de Souza</t>
+  </si>
+  <si>
+    <t>Taynara Iris de Novaes</t>
+  </si>
+  <si>
+    <t>Monica de Oliveira Liberato</t>
+  </si>
+  <si>
+    <t>Dircilaine Cristina Chinelato</t>
+  </si>
+  <si>
+    <t>Ana Carolina Monteiro de Almeida Abreu</t>
+  </si>
+  <si>
+    <t>aalbino</t>
+  </si>
+  <si>
+    <t>ralmeida</t>
+  </si>
+  <si>
+    <t>bsouza</t>
+  </si>
+  <si>
+    <t>tnovaes</t>
+  </si>
+  <si>
+    <t>mliberato</t>
+  </si>
+  <si>
+    <t>dchinelato</t>
+  </si>
+  <si>
+    <t>amonteiro</t>
+  </si>
+  <si>
+    <t>Samuel Kascher Oliveira</t>
+  </si>
+  <si>
+    <t>soliveira</t>
   </si>
 </sst>
 </file>
@@ -3156,14 +3204,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="95.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -3396,583 +3444,593 @@
         <v>94</v>
       </c>
     </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+    </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
-      </c>
-      <c r="C37" t="s">
-        <v>79</v>
-      </c>
-      <c r="D37" t="str">
-        <f>A37&amp;" "&amp;B37&amp;" "&amp;C37</f>
-        <v>CREATE USER  deliza PASSWORD '1234';</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
-      </c>
-      <c r="C38" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" t="str">
-        <f t="shared" ref="D38:D98" si="0">A38&amp;" "&amp;B38&amp;" "&amp;C38</f>
-        <v>GRANT CONNECT ON DATABASE vila_verde TO  deliza ;</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="B39" t="s">
-        <v>94</v>
-      </c>
-      <c r="C39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT USAGE ON SCHEMA integracao TO  deliza ;</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="B40" t="s">
-        <v>94</v>
-      </c>
-      <c r="C40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  deliza ;</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="B41" t="s">
-        <v>94</v>
-      </c>
-      <c r="C41" t="s">
-        <v>1</v>
-      </c>
-      <c r="D41" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  deliza ;</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO deliza ;</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="B43" t="s">
-        <v>94</v>
-      </c>
-      <c r="C43" t="s">
-        <v>1</v>
-      </c>
-      <c r="D43" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  deliza ;</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" t="s">
-        <v>1</v>
-      </c>
-      <c r="D44" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  deliza ;</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>72</v>
-      </c>
-      <c r="B45" t="s">
-        <v>94</v>
-      </c>
-      <c r="C45" t="s">
-        <v>1</v>
-      </c>
-      <c r="D45" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  deliza ;</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C46" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="D46" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  deliza ;</v>
+        <f>A46&amp;" "&amp;B46&amp;" "&amp;C46</f>
+        <v>CREATE USER  tivilaverde PASSWORD '1234';</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="B47" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C47" t="s">
         <v>1</v>
       </c>
       <c r="D47" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  deliza ;</v>
+        <f t="shared" ref="D47:D107" si="0">A47&amp;" "&amp;B47&amp;" "&amp;C47</f>
+        <v>GRANT CONNECT ON DATABASE vila_verde TO  tivilaverde ;</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B48" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  deliza ;</v>
+        <v>GRANT USAGE ON SCHEMA integracao TO  tivilaverde ;</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C49" t="s">
         <v>1</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  deliza ;</v>
+        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  tivilaverde ;</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B50" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C50" t="s">
         <v>1</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  deliza ;</v>
+        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  tivilaverde ;</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="B51" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C51" t="s">
         <v>1</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to deliza ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO tivilaverde ;</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="B52" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C52" t="s">
         <v>1</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to deliza ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  tivilaverde ;</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C53" t="s">
         <v>1</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to deliza ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  tivilaverde ;</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="B54" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C54" t="s">
         <v>1</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to deliza ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  tivilaverde ;</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="B55" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C55" t="s">
         <v>1</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to deliza ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  tivilaverde ;</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="B56" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C56" t="s">
         <v>1</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to deliza ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  tivilaverde ;</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="B57" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C57" t="s">
         <v>1</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to deliza ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  tivilaverde ;</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="B58" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C58" t="s">
         <v>1</v>
       </c>
       <c r="D58" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to deliza ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  tivilaverde ;</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="B59" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C59" t="s">
         <v>1</v>
       </c>
       <c r="D59" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to deliza ;</v>
+        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  tivilaverde ;</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B60" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C60" t="s">
         <v>1</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO deliza ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to tivilaverde ;</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B61" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C61" t="s">
         <v>1</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO deliza ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to tivilaverde ;</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="B62" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C62" t="s">
         <v>1</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  deliza ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to tivilaverde ;</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B63" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C63" t="s">
         <v>1</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO deliza ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to tivilaverde ;</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B64" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C64" t="s">
         <v>1</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO deliza ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to tivilaverde ;</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B65" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C65" t="s">
         <v>1</v>
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO deliza ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to tivilaverde ;</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B66" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C66" t="s">
         <v>1</v>
       </c>
       <c r="D66" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO deliza ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to tivilaverde ;</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B67" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C67" t="s">
         <v>1</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO deliza ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to tivilaverde ;</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="B68" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C68" t="s">
         <v>1</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  deliza ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to tivilaverde ;</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="B69" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C69" t="s">
         <v>1</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  deliza ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO tivilaverde ;</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>84</v>
+        <v>2</v>
       </c>
       <c r="B70" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C70" t="s">
         <v>1</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_leito TO  deliza ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO tivilaverde ;</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71" t="s">
+        <v>83</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  tivilaverde ;</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" t="s">
+        <v>83</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO tivilaverde ;</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" t="s">
+        <v>83</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO tivilaverde ;</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" t="s">
+        <v>83</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO tivilaverde ;</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>7</v>
+      </c>
+      <c r="B75" t="s">
+        <v>83</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO tivilaverde ;</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" t="s">
+        <v>83</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO tivilaverde ;</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>86</v>
+      </c>
+      <c r="B77" t="s">
+        <v>83</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  tivilaverde ;</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>87</v>
+      </c>
+      <c r="B78" t="s">
+        <v>83</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  tivilaverde ;</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>84</v>
+      </c>
+      <c r="B79" t="s">
+        <v>83</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.tb_leito TO  tivilaverde ;</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>85</v>
       </c>
-      <c r="B71" t="s">
-        <v>94</v>
-      </c>
-      <c r="C71" t="s">
-        <v>1</v>
-      </c>
-      <c r="D71" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  deliza ;</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D72" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D73" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D74" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D75" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D76" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D77" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D78" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D79" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>83</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1</v>
+      </c>
       <c r="D80" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
+        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  tivilaverde ;</v>
       </c>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.25">
@@ -4079,6 +4137,60 @@
     </row>
     <row r="98" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D98" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D100" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D101" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D102" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D103" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D104" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D105" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D106" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  </v>
+      </c>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D107" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  </v>
       </c>

</xml_diff>

<commit_message>
Novos filtros para gestão de leitos.
</commit_message>
<xml_diff>
--- a/script_base_dados/grants.xlsx
+++ b/script_base_dados/grants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\integracao\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D752F44-E061-4D33-A660-FEB3EF95D2BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E912C4-5962-4F7A-9B60-5E511014A0FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="116">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -368,6 +368,21 @@
   </si>
   <si>
     <t>soliveira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT SELECT on integracao.tb_crtr_intnc TO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT SELECT on integracao.tb_dieta TO </t>
+  </si>
+  <si>
+    <t>administrativo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT SELECT on integracao.tb_const TO </t>
+  </si>
+  <si>
+    <t>evaldo</t>
   </si>
 </sst>
 </file>
@@ -3204,9 +3219,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
-  <dimension ref="A1:D107"/>
+  <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3534,7 +3551,7 @@
         <v>1</v>
       </c>
       <c r="D47" t="str">
-        <f t="shared" ref="D47:D107" si="0">A47&amp;" "&amp;B47&amp;" "&amp;C47</f>
+        <f t="shared" ref="D47:D113" si="0">A47&amp;" "&amp;B47&amp;" "&amp;C47</f>
         <v>GRANT CONNECT ON DATABASE vila_verde TO  tivilaverde ;</v>
       </c>
     </row>
@@ -4033,166 +4050,646 @@
         <v>GRANT SELECT on integracao.vw_ctrl_leito TO  tivilaverde ;</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>111</v>
+      </c>
+      <c r="B81" t="s">
+        <v>115</v>
+      </c>
       <c r="D81" t="str">
         <f t="shared" si="0"/>
+        <v xml:space="preserve">GRANT SELECT on integracao.tb_crtr_intnc TO  evaldo </v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>112</v>
+      </c>
+      <c r="B82" t="s">
+        <v>115</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">GRANT SELECT on integracao.tb_dieta TO  evaldo </v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>114</v>
+      </c>
+      <c r="B83" t="s">
+        <v>115</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">GRANT SELECT on integracao.tb_const TO  evaldo </v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D86" t="str">
+        <f t="shared" si="0"/>
         <v xml:space="preserve">  </v>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D82" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D83" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D84" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D85" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D86" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>114</v>
+      </c>
+      <c r="B87" t="s">
+        <v>44</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1</v>
+      </c>
       <c r="D87" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  aoliveira ;</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>114</v>
+      </c>
+      <c r="B88" t="s">
+        <v>45</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1</v>
+      </c>
       <c r="D88" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  dalves ;</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>114</v>
+      </c>
+      <c r="B89" t="s">
+        <v>46</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1</v>
+      </c>
       <c r="D89" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  emenezes ;</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>114</v>
+      </c>
+      <c r="B90" t="s">
+        <v>47</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1</v>
+      </c>
       <c r="D90" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  gcassia ;</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>114</v>
+      </c>
+      <c r="B91" t="s">
+        <v>48</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1</v>
+      </c>
       <c r="D91" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  lmaria ;</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>114</v>
+      </c>
+      <c r="B92" t="s">
+        <v>53</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1</v>
+      </c>
       <c r="D92" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  mrezende ;</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>114</v>
+      </c>
+      <c r="B93" t="s">
+        <v>49</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1</v>
+      </c>
       <c r="D93" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  lvieira ;</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>114</v>
+      </c>
+      <c r="B94" t="s">
+        <v>54</v>
+      </c>
+      <c r="C94" t="s">
+        <v>1</v>
+      </c>
       <c r="D94" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  tsilva ;</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>114</v>
+      </c>
+      <c r="B95" t="s">
+        <v>50</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1</v>
+      </c>
       <c r="D95" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  vrodrigues ;</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>114</v>
+      </c>
+      <c r="B96" t="s">
+        <v>51</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1</v>
+      </c>
       <c r="D96" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  vlucia ;</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>114</v>
+      </c>
+      <c r="B97" t="s">
+        <v>55</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1</v>
+      </c>
       <c r="D97" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  vsilva ;</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>114</v>
+      </c>
+      <c r="B98" t="s">
+        <v>56</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1</v>
+      </c>
       <c r="D98" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  woliveira ;</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>114</v>
+      </c>
+      <c r="B99" t="s">
+        <v>52</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1</v>
+      </c>
       <c r="D99" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  wquetz ;</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>114</v>
+      </c>
+      <c r="B100" t="s">
+        <v>30</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1</v>
+      </c>
       <c r="D100" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  ftesta ;</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>114</v>
+      </c>
+      <c r="B101" t="s">
+        <v>59</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1</v>
+      </c>
       <c r="D101" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  simone ;</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>114</v>
+      </c>
+      <c r="B102" t="s">
+        <v>61</v>
+      </c>
+      <c r="C102" t="s">
+        <v>1</v>
+      </c>
       <c r="D102" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  grazielle ;</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>114</v>
+      </c>
+      <c r="B103" t="s">
+        <v>63</v>
+      </c>
+      <c r="C103" t="s">
+        <v>1</v>
+      </c>
       <c r="D103" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  dayane ;</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>114</v>
+      </c>
+      <c r="B104" t="s">
+        <v>65</v>
+      </c>
+      <c r="C104" t="s">
+        <v>1</v>
+      </c>
       <c r="D104" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  ronan ;</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>114</v>
+      </c>
+      <c r="B105" t="s">
+        <v>10</v>
+      </c>
+      <c r="C105" t="s">
+        <v>1</v>
+      </c>
       <c r="D105" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  clovismelo ;</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>114</v>
+      </c>
+      <c r="B106" t="s">
+        <v>11</v>
+      </c>
+      <c r="C106" t="s">
+        <v>1</v>
+      </c>
       <c r="D106" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+        <v>GRANT SELECT on integracao.tb_const TO  mariabethania ;</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>114</v>
+      </c>
+      <c r="B107" t="s">
+        <v>12</v>
+      </c>
+      <c r="C107" t="s">
+        <v>1</v>
+      </c>
       <c r="D107" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
+        <v>GRANT SELECT on integracao.tb_const TO  fernandazeferino ;</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>114</v>
+      </c>
+      <c r="B108" t="s">
+        <v>81</v>
+      </c>
+      <c r="C108" t="s">
+        <v>1</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.tb_const TO  camila ;</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>114</v>
+      </c>
+      <c r="B109" t="s">
+        <v>113</v>
+      </c>
+      <c r="C109" t="s">
+        <v>1</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.tb_const TO  administrativo ;</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>114</v>
+      </c>
+      <c r="B110" t="s">
+        <v>83</v>
+      </c>
+      <c r="C110" t="s">
+        <v>1</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.tb_const TO  tivilaverde ;</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>114</v>
+      </c>
+      <c r="B111" t="s">
+        <v>16</v>
+      </c>
+      <c r="C111" t="s">
+        <v>1</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.tb_const TO  lamorim ;</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>114</v>
+      </c>
+      <c r="B112" t="s">
+        <v>13</v>
+      </c>
+      <c r="C112" t="s">
+        <v>1</v>
+      </c>
+      <c r="D112" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.tb_const TO  mvilela ;</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>114</v>
+      </c>
+      <c r="B113" t="s">
+        <v>14</v>
+      </c>
+      <c r="C113" t="s">
+        <v>1</v>
+      </c>
+      <c r="D113" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.tb_const TO  fcampos ;</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>114</v>
+      </c>
+      <c r="B114" t="s">
+        <v>15</v>
+      </c>
+      <c r="C114" t="s">
+        <v>1</v>
+      </c>
+      <c r="D114" t="str">
+        <f t="shared" ref="D114:D126" si="1">A114&amp;" "&amp;B114&amp;" "&amp;C114</f>
+        <v>GRANT SELECT on integracao.tb_const TO  bcorrea ;</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>9</v>
+      </c>
+      <c r="C115" t="s">
+        <v>1</v>
+      </c>
+      <c r="D115" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.tb_const TO  mmattos ;</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>114</v>
+      </c>
+      <c r="B116" t="s">
+        <v>92</v>
+      </c>
+      <c r="C116" t="s">
+        <v>1</v>
+      </c>
+      <c r="D116" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.tb_const TO  greis ;</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>114</v>
+      </c>
+      <c r="B117" t="s">
+        <v>93</v>
+      </c>
+      <c r="C117" t="s">
+        <v>1</v>
+      </c>
+      <c r="D117" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.tb_const TO  ldelgado ;</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>114</v>
+      </c>
+      <c r="B118" t="s">
+        <v>94</v>
+      </c>
+      <c r="C118" t="s">
+        <v>1</v>
+      </c>
+      <c r="D118" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.tb_const TO  deliza ;</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>114</v>
+      </c>
+      <c r="B119" t="s">
+        <v>102</v>
+      </c>
+      <c r="C119" t="s">
+        <v>1</v>
+      </c>
+      <c r="D119" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.tb_const TO  aalbino ;</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>114</v>
+      </c>
+      <c r="B120" t="s">
+        <v>103</v>
+      </c>
+      <c r="C120" t="s">
+        <v>1</v>
+      </c>
+      <c r="D120" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.tb_const TO  ralmeida ;</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>114</v>
+      </c>
+      <c r="B121" t="s">
+        <v>104</v>
+      </c>
+      <c r="C121" t="s">
+        <v>1</v>
+      </c>
+      <c r="D121" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.tb_const TO  bsouza ;</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>114</v>
+      </c>
+      <c r="B122" t="s">
+        <v>105</v>
+      </c>
+      <c r="C122" t="s">
+        <v>1</v>
+      </c>
+      <c r="D122" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.tb_const TO  tnovaes ;</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>114</v>
+      </c>
+      <c r="B123" t="s">
+        <v>106</v>
+      </c>
+      <c r="C123" t="s">
+        <v>1</v>
+      </c>
+      <c r="D123" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.tb_const TO  mliberato ;</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>114</v>
+      </c>
+      <c r="B124" t="s">
+        <v>107</v>
+      </c>
+      <c r="C124" t="s">
+        <v>1</v>
+      </c>
+      <c r="D124" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.tb_const TO  dchinelato ;</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>114</v>
+      </c>
+      <c r="B125" t="s">
+        <v>108</v>
+      </c>
+      <c r="C125" t="s">
+        <v>1</v>
+      </c>
+      <c r="D125" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.tb_const TO  amonteiro ;</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>114</v>
+      </c>
+      <c r="B126" t="s">
+        <v>110</v>
+      </c>
+      <c r="C126" t="s">
+        <v>1</v>
+      </c>
+      <c r="D126" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.tb_const TO  soliveira ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalização dos relatórios de bmh_online.php
</commit_message>
<xml_diff>
--- a/script_base_dados/grants.xlsx
+++ b/script_base_dados/grants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\integracao\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E912C4-5962-4F7A-9B60-5E511014A0FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7AB033-626F-4832-9299-6568ADB3354C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="139">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -382,7 +382,76 @@
     <t xml:space="preserve">GRANT SELECT on integracao.tb_const TO </t>
   </si>
   <si>
-    <t>evaldo</t>
+    <t>Amata Xavier Medeiros,</t>
+  </si>
+  <si>
+    <t>Otávio Pacheco Pamplona Corte Real,</t>
+  </si>
+  <si>
+    <t>Fernanda Medeiros Viglioni,</t>
+  </si>
+  <si>
+    <t>Stephanie S.F. Bhering dos Santos,</t>
+  </si>
+  <si>
+    <t>Vivian de Andrade Hauck Pinto</t>
+  </si>
+  <si>
+    <t>Daniela Fajardo Cury Gogliath,</t>
+  </si>
+  <si>
+    <t>João Vitor Miguel da Silva</t>
+  </si>
+  <si>
+    <t>Cassio de Oliveira Brugiolo</t>
+  </si>
+  <si>
+    <t>Pedro Ferrreira Brito Franco Lessa</t>
+  </si>
+  <si>
+    <t>Ademir Azevedo Morais</t>
+  </si>
+  <si>
+    <t>Pamela Karine de Oliveira Vargas,</t>
+  </si>
+  <si>
+    <t>axavier</t>
+  </si>
+  <si>
+    <t>opacheco</t>
+  </si>
+  <si>
+    <t>fmedeiros</t>
+  </si>
+  <si>
+    <t>dfajardo</t>
+  </si>
+  <si>
+    <t>sbhering</t>
+  </si>
+  <si>
+    <t>vandrade</t>
+  </si>
+  <si>
+    <t>jmiguel</t>
+  </si>
+  <si>
+    <t>coliveira</t>
+  </si>
+  <si>
+    <t>pferreira</t>
+  </si>
+  <si>
+    <t>amorais</t>
+  </si>
+  <si>
+    <t>poliveira</t>
+  </si>
+  <si>
+    <t>farmacia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT SELECT on integracao.vw_bmh_online TO </t>
   </si>
 </sst>
 </file>
@@ -3219,10 +3288,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
-  <dimension ref="A1:D126"/>
+  <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100:D151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3445,7 +3514,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -3453,7 +3522,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>91</v>
       </c>
@@ -3461,7 +3530,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -3469,7 +3538,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -3477,7 +3546,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -3485,7 +3554,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>98</v>
       </c>
@@ -3493,7 +3562,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>99</v>
       </c>
@@ -3501,7 +3570,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>100</v>
       </c>
@@ -3509,7 +3578,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>101</v>
       </c>
@@ -3517,7 +3586,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>109</v>
       </c>
@@ -3525,706 +3594,652 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>78</v>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
-      </c>
-      <c r="C46" t="s">
-        <v>79</v>
-      </c>
-      <c r="D46" t="str">
-        <f>A46&amp;" "&amp;B46&amp;" "&amp;C46</f>
-        <v>CREATE USER  tivilaverde PASSWORD '1234';</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>88</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
-      </c>
-      <c r="C47" t="s">
-        <v>1</v>
-      </c>
-      <c r="D47" t="str">
-        <f t="shared" ref="D47:D113" si="0">A47&amp;" "&amp;B47&amp;" "&amp;C47</f>
-        <v>GRANT CONNECT ON DATABASE vila_verde TO  tivilaverde ;</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>66</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="B48" t="s">
-        <v>83</v>
-      </c>
-      <c r="C48" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT USAGE ON SCHEMA integracao TO  tivilaverde ;</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>67</v>
+      <c r="A49" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B49" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" t="s">
-        <v>1</v>
-      </c>
-      <c r="D49" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  tivilaverde ;</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>68</v>
+      <c r="A50" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="B50" t="s">
-        <v>83</v>
-      </c>
-      <c r="C50" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  tivilaverde ;</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>69</v>
+      <c r="A51" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="B51" t="s">
-        <v>83</v>
-      </c>
-      <c r="C51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D51" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO tivilaverde ;</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>70</v>
+      <c r="A52" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
-      </c>
-      <c r="C52" t="s">
-        <v>1</v>
-      </c>
-      <c r="D52" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  tivilaverde ;</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>71</v>
+      <c r="A53" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="B53" t="s">
-        <v>83</v>
-      </c>
-      <c r="C53" t="s">
-        <v>1</v>
-      </c>
-      <c r="D53" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  tivilaverde ;</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>72</v>
+      <c r="A54" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="B54" t="s">
-        <v>83</v>
-      </c>
-      <c r="C54" t="s">
-        <v>1</v>
-      </c>
-      <c r="D54" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  tivilaverde ;</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>73</v>
+      <c r="A55" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
-      </c>
-      <c r="C55" t="s">
-        <v>1</v>
-      </c>
-      <c r="D55" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  tivilaverde ;</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>74</v>
+      <c r="A56" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="B56" t="s">
-        <v>83</v>
-      </c>
-      <c r="C56" t="s">
-        <v>1</v>
-      </c>
-      <c r="D56" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  tivilaverde ;</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>75</v>
-      </c>
       <c r="B57" t="s">
-        <v>83</v>
-      </c>
-      <c r="C57" t="s">
-        <v>1</v>
-      </c>
-      <c r="D57" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  tivilaverde ;</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>76</v>
-      </c>
-      <c r="B58" t="s">
-        <v>83</v>
-      </c>
-      <c r="C58" t="s">
-        <v>1</v>
-      </c>
-      <c r="D58" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  tivilaverde ;</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B59" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C59" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="D59" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  tivilaverde ;</v>
+        <f>A59&amp;" "&amp;B59&amp;" "&amp;C59</f>
+        <v>CREATE USER  farmacia PASSWORD '1234';</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="B60" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C60" t="s">
         <v>1</v>
       </c>
       <c r="D60" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to tivilaverde ;</v>
+        <f t="shared" ref="D60:D126" si="0">A60&amp;" "&amp;B60&amp;" "&amp;C60</f>
+        <v>GRANT CONNECT ON DATABASE vila_verde TO  farmacia ;</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="B61" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C61" t="s">
         <v>1</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to tivilaverde ;</v>
+        <v>GRANT USAGE ON SCHEMA integracao TO  farmacia ;</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="B62" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C62" t="s">
         <v>1</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to tivilaverde ;</v>
+        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  farmacia ;</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="B63" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C63" t="s">
         <v>1</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to tivilaverde ;</v>
+        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  farmacia ;</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="B64" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C64" t="s">
         <v>1</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to tivilaverde ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO farmacia ;</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="B65" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C65" t="s">
         <v>1</v>
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to tivilaverde ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  farmacia ;</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="B66" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C66" t="s">
         <v>1</v>
       </c>
       <c r="D66" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to tivilaverde ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  farmacia ;</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="B67" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C67" t="s">
         <v>1</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to tivilaverde ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  farmacia ;</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="B68" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C68" t="s">
         <v>1</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to tivilaverde ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  farmacia ;</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="B69" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C69" t="s">
         <v>1</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO tivilaverde ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  farmacia ;</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="B70" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C70" t="s">
         <v>1</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO tivilaverde ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  farmacia ;</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>3</v>
+        <v>76</v>
       </c>
       <c r="B71" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C71" t="s">
         <v>1</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  tivilaverde ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  farmacia ;</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="B72" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C72" t="s">
         <v>1</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO tivilaverde ;</v>
+        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  farmacia ;</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B73" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C73" t="s">
         <v>1</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO tivilaverde ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to farmacia ;</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B74" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C74" t="s">
         <v>1</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO tivilaverde ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to farmacia ;</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B75" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C75" t="s">
         <v>1</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO tivilaverde ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to farmacia ;</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B76" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C76" t="s">
         <v>1</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO tivilaverde ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to farmacia ;</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="B77" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  tivilaverde ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to farmacia ;</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="B78" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C78" t="s">
         <v>1</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  tivilaverde ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to farmacia ;</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="B79" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C79" t="s">
         <v>1</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_leito TO  tivilaverde ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to farmacia ;</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="B80" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C80" t="s">
         <v>1</v>
       </c>
       <c r="D80" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  tivilaverde ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to farmacia ;</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="B81" t="s">
-        <v>115</v>
+        <v>137</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">GRANT SELECT on integracao.tb_crtr_intnc TO  evaldo </v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to farmacia ;</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>112</v>
+        <v>0</v>
       </c>
       <c r="B82" t="s">
-        <v>115</v>
+        <v>137</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">GRANT SELECT on integracao.tb_dieta TO  evaldo </v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO farmacia ;</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>114</v>
+        <v>2</v>
       </c>
       <c r="B83" t="s">
-        <v>115</v>
+        <v>137</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1</v>
       </c>
       <c r="D83" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">GRANT SELECT on integracao.tb_const TO  evaldo </v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO farmacia ;</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84" t="s">
+        <v>137</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  farmacia ;</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>4</v>
+      </c>
+      <c r="B85" t="s">
+        <v>137</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO farmacia ;</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86" t="s">
+        <v>137</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1</v>
+      </c>
       <c r="D86" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO farmacia ;</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>114</v>
+        <v>6</v>
       </c>
       <c r="B87" t="s">
-        <v>44</v>
+        <v>137</v>
       </c>
       <c r="C87" t="s">
         <v>1</v>
       </c>
       <c r="D87" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  aoliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO farmacia ;</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="B88" t="s">
-        <v>45</v>
+        <v>137</v>
       </c>
       <c r="C88" t="s">
         <v>1</v>
       </c>
       <c r="D88" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  dalves ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO farmacia ;</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>114</v>
+        <v>8</v>
       </c>
       <c r="B89" t="s">
-        <v>46</v>
+        <v>137</v>
       </c>
       <c r="C89" t="s">
         <v>1</v>
       </c>
       <c r="D89" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  emenezes ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO farmacia ;</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="B90" t="s">
-        <v>47</v>
+        <v>137</v>
       </c>
       <c r="C90" t="s">
         <v>1</v>
       </c>
       <c r="D90" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  gcassia ;</v>
+        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  farmacia ;</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="B91" t="s">
-        <v>48</v>
+        <v>137</v>
       </c>
       <c r="C91" t="s">
         <v>1</v>
       </c>
       <c r="D91" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  lmaria ;</v>
+        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  farmacia ;</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
       <c r="B92" t="s">
-        <v>53</v>
+        <v>137</v>
       </c>
       <c r="C92" t="s">
         <v>1</v>
       </c>
       <c r="D92" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  mrezende ;</v>
+        <v>GRANT SELECT on integracao.tb_leito TO  farmacia ;</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="B93" t="s">
-        <v>49</v>
+        <v>137</v>
       </c>
       <c r="C93" t="s">
         <v>1</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  lvieira ;</v>
+        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  farmacia ;</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B94" t="s">
-        <v>54</v>
+        <v>137</v>
       </c>
       <c r="C94" t="s">
         <v>1</v>
       </c>
       <c r="D94" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  tsilva ;</v>
+        <v>GRANT SELECT on integracao.tb_crtr_intnc TO  farmacia ;</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B95" t="s">
-        <v>50</v>
+        <v>137</v>
       </c>
       <c r="C95" t="s">
         <v>1</v>
       </c>
       <c r="D95" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  vrodrigues ;</v>
+        <v>GRANT SELECT on integracao.tb_dieta TO  farmacia ;</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4232,464 +4247,800 @@
         <v>114</v>
       </c>
       <c r="B96" t="s">
-        <v>51</v>
+        <v>137</v>
       </c>
       <c r="C96" t="s">
         <v>1</v>
       </c>
       <c r="D96" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  vlucia ;</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>114</v>
-      </c>
-      <c r="B97" t="s">
-        <v>55</v>
-      </c>
-      <c r="C97" t="s">
-        <v>1</v>
-      </c>
-      <c r="D97" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  vsilva ;</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>114</v>
-      </c>
-      <c r="B98" t="s">
-        <v>56</v>
-      </c>
-      <c r="C98" t="s">
-        <v>1</v>
-      </c>
-      <c r="D98" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  woliveira ;</v>
+        <v>GRANT SELECT on integracao.tb_const TO  farmacia ;</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>114</v>
-      </c>
-      <c r="B99" t="s">
-        <v>52</v>
-      </c>
-      <c r="C99" t="s">
-        <v>1</v>
-      </c>
       <c r="D99" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  wquetz ;</v>
+        <v xml:space="preserve">  </v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B100" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C100" t="s">
         <v>1</v>
       </c>
       <c r="D100" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  ftesta ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  aoliveira ;</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B101" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C101" t="s">
         <v>1</v>
       </c>
       <c r="D101" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  simone ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  dalves ;</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B102" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C102" t="s">
         <v>1</v>
       </c>
       <c r="D102" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  grazielle ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  emenezes ;</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B103" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C103" t="s">
         <v>1</v>
       </c>
       <c r="D103" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  dayane ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  gcassia ;</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B104" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C104" t="s">
         <v>1</v>
       </c>
       <c r="D104" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  ronan ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  lmaria ;</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B105" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="C105" t="s">
         <v>1</v>
       </c>
       <c r="D105" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  clovismelo ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  mrezende ;</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B106" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="C106" t="s">
         <v>1</v>
       </c>
       <c r="D106" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  mariabethania ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  lvieira ;</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B107" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="C107" t="s">
         <v>1</v>
       </c>
       <c r="D107" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  fernandazeferino ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  tsilva ;</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B108" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="C108" t="s">
         <v>1</v>
       </c>
       <c r="D108" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  camila ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  vrodrigues ;</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B109" t="s">
-        <v>113</v>
+        <v>51</v>
       </c>
       <c r="C109" t="s">
         <v>1</v>
       </c>
       <c r="D109" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  administrativo ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  vlucia ;</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B110" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C110" t="s">
         <v>1</v>
       </c>
       <c r="D110" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  tivilaverde ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  vsilva ;</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B111" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C111" t="s">
         <v>1</v>
       </c>
       <c r="D111" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  lamorim ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  woliveira ;</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B112" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="C112" t="s">
         <v>1</v>
       </c>
       <c r="D112" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  mvilela ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  wquetz ;</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B113" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C113" t="s">
         <v>1</v>
       </c>
       <c r="D113" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  fcampos ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  ftesta ;</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B114" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="C114" t="s">
         <v>1</v>
       </c>
       <c r="D114" t="str">
-        <f t="shared" ref="D114:D126" si="1">A114&amp;" "&amp;B114&amp;" "&amp;C114</f>
-        <v>GRANT SELECT on integracao.tb_const TO  bcorrea ;</v>
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  simone ;</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B115" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="C115" t="s">
         <v>1</v>
       </c>
       <c r="D115" t="str">
-        <f t="shared" si="1"/>
-        <v>GRANT SELECT on integracao.tb_const TO  mmattos ;</v>
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  grazielle ;</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B116" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="C116" t="s">
         <v>1</v>
       </c>
       <c r="D116" t="str">
-        <f t="shared" si="1"/>
-        <v>GRANT SELECT on integracao.tb_const TO  greis ;</v>
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  dayane ;</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B117" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="C117" t="s">
         <v>1</v>
       </c>
       <c r="D117" t="str">
-        <f t="shared" si="1"/>
-        <v>GRANT SELECT on integracao.tb_const TO  ldelgado ;</v>
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  ronan ;</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B118" t="s">
-        <v>94</v>
+        <v>10</v>
       </c>
       <c r="C118" t="s">
         <v>1</v>
       </c>
       <c r="D118" t="str">
-        <f t="shared" si="1"/>
-        <v>GRANT SELECT on integracao.tb_const TO  deliza ;</v>
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  clovismelo ;</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B119" t="s">
-        <v>102</v>
+        <v>11</v>
       </c>
       <c r="C119" t="s">
         <v>1</v>
       </c>
       <c r="D119" t="str">
-        <f t="shared" si="1"/>
-        <v>GRANT SELECT on integracao.tb_const TO  aalbino ;</v>
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  mariabethania ;</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B120" t="s">
-        <v>103</v>
+        <v>12</v>
       </c>
       <c r="C120" t="s">
         <v>1</v>
       </c>
       <c r="D120" t="str">
-        <f t="shared" si="1"/>
-        <v>GRANT SELECT on integracao.tb_const TO  ralmeida ;</v>
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  fernandazeferino ;</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B121" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="C121" t="s">
         <v>1</v>
       </c>
       <c r="D121" t="str">
-        <f t="shared" si="1"/>
-        <v>GRANT SELECT on integracao.tb_const TO  bsouza ;</v>
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  camila ;</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B122" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C122" t="s">
         <v>1</v>
       </c>
       <c r="D122" t="str">
-        <f t="shared" si="1"/>
-        <v>GRANT SELECT on integracao.tb_const TO  tnovaes ;</v>
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  administrativo ;</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B123" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C123" t="s">
         <v>1</v>
       </c>
       <c r="D123" t="str">
-        <f t="shared" si="1"/>
-        <v>GRANT SELECT on integracao.tb_const TO  mliberato ;</v>
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  tivilaverde ;</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B124" t="s">
-        <v>107</v>
+        <v>16</v>
       </c>
       <c r="C124" t="s">
         <v>1</v>
       </c>
       <c r="D124" t="str">
-        <f t="shared" si="1"/>
-        <v>GRANT SELECT on integracao.tb_const TO  dchinelato ;</v>
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  lamorim ;</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B125" t="s">
-        <v>108</v>
+        <v>13</v>
       </c>
       <c r="C125" t="s">
         <v>1</v>
       </c>
       <c r="D125" t="str">
-        <f t="shared" si="1"/>
-        <v>GRANT SELECT on integracao.tb_const TO  amonteiro ;</v>
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  mvilela ;</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B126" t="s">
+        <v>14</v>
+      </c>
+      <c r="C126" t="s">
+        <v>1</v>
+      </c>
+      <c r="D126" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  fcampos ;</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>138</v>
+      </c>
+      <c r="B127" t="s">
+        <v>15</v>
+      </c>
+      <c r="C127" t="s">
+        <v>1</v>
+      </c>
+      <c r="D127" t="str">
+        <f t="shared" ref="D127:D151" si="1">A127&amp;" "&amp;B127&amp;" "&amp;C127</f>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  bcorrea ;</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>138</v>
+      </c>
+      <c r="B128" t="s">
+        <v>9</v>
+      </c>
+      <c r="C128" t="s">
+        <v>1</v>
+      </c>
+      <c r="D128" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  mmattos ;</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>138</v>
+      </c>
+      <c r="B129" t="s">
+        <v>92</v>
+      </c>
+      <c r="C129" t="s">
+        <v>1</v>
+      </c>
+      <c r="D129" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  greis ;</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>138</v>
+      </c>
+      <c r="B130" t="s">
+        <v>93</v>
+      </c>
+      <c r="C130" t="s">
+        <v>1</v>
+      </c>
+      <c r="D130" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  ldelgado ;</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>138</v>
+      </c>
+      <c r="B131" t="s">
+        <v>94</v>
+      </c>
+      <c r="C131" t="s">
+        <v>1</v>
+      </c>
+      <c r="D131" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  deliza ;</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>138</v>
+      </c>
+      <c r="B132" t="s">
+        <v>102</v>
+      </c>
+      <c r="C132" t="s">
+        <v>1</v>
+      </c>
+      <c r="D132" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  aalbino ;</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>138</v>
+      </c>
+      <c r="B133" t="s">
+        <v>103</v>
+      </c>
+      <c r="C133" t="s">
+        <v>1</v>
+      </c>
+      <c r="D133" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  ralmeida ;</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>138</v>
+      </c>
+      <c r="B134" t="s">
+        <v>104</v>
+      </c>
+      <c r="C134" t="s">
+        <v>1</v>
+      </c>
+      <c r="D134" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  bsouza ;</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>138</v>
+      </c>
+      <c r="B135" t="s">
+        <v>105</v>
+      </c>
+      <c r="C135" t="s">
+        <v>1</v>
+      </c>
+      <c r="D135" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  tnovaes ;</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>138</v>
+      </c>
+      <c r="B136" t="s">
+        <v>106</v>
+      </c>
+      <c r="C136" t="s">
+        <v>1</v>
+      </c>
+      <c r="D136" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  mliberato ;</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>138</v>
+      </c>
+      <c r="B137" t="s">
+        <v>107</v>
+      </c>
+      <c r="C137" t="s">
+        <v>1</v>
+      </c>
+      <c r="D137" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  dchinelato ;</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>138</v>
+      </c>
+      <c r="B138" t="s">
+        <v>108</v>
+      </c>
+      <c r="C138" t="s">
+        <v>1</v>
+      </c>
+      <c r="D138" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  amonteiro ;</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
         <v>110</v>
       </c>
-      <c r="C126" t="s">
-        <v>1</v>
-      </c>
-      <c r="D126" t="str">
+      <c r="C139" t="s">
+        <v>1</v>
+      </c>
+      <c r="D139" t="str">
         <f t="shared" si="1"/>
-        <v>GRANT SELECT on integracao.tb_const TO  soliveira ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  soliveira ;</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>138</v>
+      </c>
+      <c r="B140" t="s">
+        <v>126</v>
+      </c>
+      <c r="C140" t="s">
+        <v>1</v>
+      </c>
+      <c r="D140" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  axavier ;</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>138</v>
+      </c>
+      <c r="B141" t="s">
+        <v>127</v>
+      </c>
+      <c r="C141" t="s">
+        <v>1</v>
+      </c>
+      <c r="D141" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  opacheco ;</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>138</v>
+      </c>
+      <c r="B142" t="s">
+        <v>128</v>
+      </c>
+      <c r="C142" t="s">
+        <v>1</v>
+      </c>
+      <c r="D142" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  fmedeiros ;</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>138</v>
+      </c>
+      <c r="B143" t="s">
+        <v>130</v>
+      </c>
+      <c r="C143" t="s">
+        <v>1</v>
+      </c>
+      <c r="D143" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  sbhering ;</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>138</v>
+      </c>
+      <c r="B144" t="s">
+        <v>131</v>
+      </c>
+      <c r="C144" t="s">
+        <v>1</v>
+      </c>
+      <c r="D144" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  vandrade ;</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>138</v>
+      </c>
+      <c r="B145" t="s">
+        <v>129</v>
+      </c>
+      <c r="C145" t="s">
+        <v>1</v>
+      </c>
+      <c r="D145" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  dfajardo ;</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>138</v>
+      </c>
+      <c r="B146" t="s">
+        <v>132</v>
+      </c>
+      <c r="C146" t="s">
+        <v>1</v>
+      </c>
+      <c r="D146" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  jmiguel ;</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>138</v>
+      </c>
+      <c r="B147" t="s">
+        <v>133</v>
+      </c>
+      <c r="C147" t="s">
+        <v>1</v>
+      </c>
+      <c r="D147" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  coliveira ;</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>138</v>
+      </c>
+      <c r="B148" t="s">
+        <v>134</v>
+      </c>
+      <c r="C148" t="s">
+        <v>1</v>
+      </c>
+      <c r="D148" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  pferreira ;</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>138</v>
+      </c>
+      <c r="B149" t="s">
+        <v>135</v>
+      </c>
+      <c r="C149" t="s">
+        <v>1</v>
+      </c>
+      <c r="D149" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  amorais ;</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>138</v>
+      </c>
+      <c r="B150" t="s">
+        <v>136</v>
+      </c>
+      <c r="C150" t="s">
+        <v>1</v>
+      </c>
+      <c r="D150" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  poliveira ;</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>138</v>
+      </c>
+      <c r="B151" t="s">
+        <v>137</v>
+      </c>
+      <c r="C151" t="s">
+        <v>1</v>
+      </c>
+      <c r="D151" t="str">
+        <f t="shared" si="1"/>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  farmacia ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Criação da funcionalidade de Alteração do Destino de Alta
</commit_message>
<xml_diff>
--- a/script_base_dados/grants.xlsx
+++ b/script_base_dados/grants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\integracao\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7AB033-626F-4832-9299-6568ADB3354C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE671D1-3C26-4D28-ADCC-17123181BDE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="140">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -452,6 +452,9 @@
   </si>
   <si>
     <t xml:space="preserve">GRANT SELECT on integracao.vw_bmh_online TO </t>
+  </si>
+  <si>
+    <t>flavia</t>
   </si>
 </sst>
 </file>
@@ -3290,9 +3293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
   <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100:D151"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3692,14 +3693,14 @@
         <v>78</v>
       </c>
       <c r="B59" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C59" t="s">
         <v>79</v>
       </c>
       <c r="D59" t="str">
         <f>A59&amp;" "&amp;B59&amp;" "&amp;C59</f>
-        <v>CREATE USER  farmacia PASSWORD '1234';</v>
+        <v>CREATE USER  flavia PASSWORD '1234';</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3707,14 +3708,14 @@
         <v>88</v>
       </c>
       <c r="B60" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C60" t="s">
         <v>1</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" ref="D60:D126" si="0">A60&amp;" "&amp;B60&amp;" "&amp;C60</f>
-        <v>GRANT CONNECT ON DATABASE vila_verde TO  farmacia ;</v>
+        <v>GRANT CONNECT ON DATABASE vila_verde TO  flavia ;</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3722,14 +3723,14 @@
         <v>66</v>
       </c>
       <c r="B61" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C61" t="s">
         <v>1</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT USAGE ON SCHEMA integracao TO  farmacia ;</v>
+        <v>GRANT USAGE ON SCHEMA integracao TO  flavia ;</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3737,14 +3738,14 @@
         <v>67</v>
       </c>
       <c r="B62" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C62" t="s">
         <v>1</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  farmacia ;</v>
+        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  flavia ;</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3752,14 +3753,14 @@
         <v>68</v>
       </c>
       <c r="B63" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C63" t="s">
         <v>1</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  farmacia ;</v>
+        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  flavia ;</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3767,14 +3768,14 @@
         <v>69</v>
       </c>
       <c r="B64" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C64" t="s">
         <v>1</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO farmacia ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO flavia ;</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3782,14 +3783,14 @@
         <v>70</v>
       </c>
       <c r="B65" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C65" t="s">
         <v>1</v>
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  farmacia ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  flavia ;</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3797,14 +3798,14 @@
         <v>71</v>
       </c>
       <c r="B66" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C66" t="s">
         <v>1</v>
       </c>
       <c r="D66" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  farmacia ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  flavia ;</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3812,14 +3813,14 @@
         <v>72</v>
       </c>
       <c r="B67" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C67" t="s">
         <v>1</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  farmacia ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  flavia ;</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3827,14 +3828,14 @@
         <v>73</v>
       </c>
       <c r="B68" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C68" t="s">
         <v>1</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  farmacia ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  flavia ;</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3842,14 +3843,14 @@
         <v>74</v>
       </c>
       <c r="B69" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C69" t="s">
         <v>1</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  farmacia ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  flavia ;</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3857,14 +3858,14 @@
         <v>75</v>
       </c>
       <c r="B70" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C70" t="s">
         <v>1</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  farmacia ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  flavia ;</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3872,14 +3873,14 @@
         <v>76</v>
       </c>
       <c r="B71" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C71" t="s">
         <v>1</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  farmacia ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  flavia ;</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3887,14 +3888,14 @@
         <v>77</v>
       </c>
       <c r="B72" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C72" t="s">
         <v>1</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  farmacia ;</v>
+        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  flavia ;</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3902,14 +3903,14 @@
         <v>27</v>
       </c>
       <c r="B73" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C73" t="s">
         <v>1</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to farmacia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to flavia ;</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3917,14 +3918,14 @@
         <v>25</v>
       </c>
       <c r="B74" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C74" t="s">
         <v>1</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to farmacia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to flavia ;</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3932,14 +3933,14 @@
         <v>26</v>
       </c>
       <c r="B75" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C75" t="s">
         <v>1</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to farmacia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to flavia ;</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3947,14 +3948,14 @@
         <v>19</v>
       </c>
       <c r="B76" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C76" t="s">
         <v>1</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to farmacia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to flavia ;</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3962,14 +3963,14 @@
         <v>20</v>
       </c>
       <c r="B77" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to farmacia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to flavia ;</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -3977,14 +3978,14 @@
         <v>21</v>
       </c>
       <c r="B78" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C78" t="s">
         <v>1</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to farmacia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to flavia ;</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -3992,14 +3993,14 @@
         <v>22</v>
       </c>
       <c r="B79" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C79" t="s">
         <v>1</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to farmacia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to flavia ;</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4007,14 +4008,14 @@
         <v>23</v>
       </c>
       <c r="B80" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C80" t="s">
         <v>1</v>
       </c>
       <c r="D80" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to farmacia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to flavia ;</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -4022,14 +4023,14 @@
         <v>24</v>
       </c>
       <c r="B81" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C81" t="s">
         <v>1</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to farmacia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to flavia ;</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4037,14 +4038,14 @@
         <v>0</v>
       </c>
       <c r="B82" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C82" t="s">
         <v>1</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO farmacia ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO flavia ;</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -4052,14 +4053,14 @@
         <v>2</v>
       </c>
       <c r="B83" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C83" t="s">
         <v>1</v>
       </c>
       <c r="D83" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO farmacia ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO flavia ;</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -4067,14 +4068,14 @@
         <v>3</v>
       </c>
       <c r="B84" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C84" t="s">
         <v>1</v>
       </c>
       <c r="D84" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  farmacia ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  flavia ;</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -4082,14 +4083,14 @@
         <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C85" t="s">
         <v>1</v>
       </c>
       <c r="D85" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO farmacia ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO flavia ;</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4097,14 +4098,14 @@
         <v>5</v>
       </c>
       <c r="B86" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C86" t="s">
         <v>1</v>
       </c>
       <c r="D86" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO farmacia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO flavia ;</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4112,14 +4113,14 @@
         <v>6</v>
       </c>
       <c r="B87" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C87" t="s">
         <v>1</v>
       </c>
       <c r="D87" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO farmacia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO flavia ;</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -4127,14 +4128,14 @@
         <v>7</v>
       </c>
       <c r="B88" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C88" t="s">
         <v>1</v>
       </c>
       <c r="D88" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO farmacia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO flavia ;</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4142,14 +4143,14 @@
         <v>8</v>
       </c>
       <c r="B89" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C89" t="s">
         <v>1</v>
       </c>
       <c r="D89" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO farmacia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO flavia ;</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -4157,14 +4158,14 @@
         <v>86</v>
       </c>
       <c r="B90" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C90" t="s">
         <v>1</v>
       </c>
       <c r="D90" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  farmacia ;</v>
+        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  flavia ;</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4172,14 +4173,14 @@
         <v>87</v>
       </c>
       <c r="B91" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C91" t="s">
         <v>1</v>
       </c>
       <c r="D91" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  farmacia ;</v>
+        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  flavia ;</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4187,14 +4188,14 @@
         <v>84</v>
       </c>
       <c r="B92" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C92" t="s">
         <v>1</v>
       </c>
       <c r="D92" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_leito TO  farmacia ;</v>
+        <v>GRANT SELECT on integracao.tb_leito TO  flavia ;</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -4202,14 +4203,14 @@
         <v>85</v>
       </c>
       <c r="B93" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C93" t="s">
         <v>1</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  farmacia ;</v>
+        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  flavia ;</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4217,14 +4218,14 @@
         <v>111</v>
       </c>
       <c r="B94" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C94" t="s">
         <v>1</v>
       </c>
       <c r="D94" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_crtr_intnc TO  farmacia ;</v>
+        <v>GRANT SELECT on integracao.tb_crtr_intnc TO  flavia ;</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -4232,14 +4233,14 @@
         <v>112</v>
       </c>
       <c r="B95" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C95" t="s">
         <v>1</v>
       </c>
       <c r="D95" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_dieta TO  farmacia ;</v>
+        <v>GRANT SELECT on integracao.tb_dieta TO  flavia ;</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4247,14 +4248,14 @@
         <v>114</v>
       </c>
       <c r="B96" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C96" t="s">
         <v>1</v>
       </c>
       <c r="D96" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  farmacia ;</v>
+        <v>GRANT SELECT on integracao.tb_const TO  flavia ;</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Atualização da mudança de leito para carregar todos os dados.
</commit_message>
<xml_diff>
--- a/script_base_dados/grants.xlsx
+++ b/script_base_dados/grants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\integracao\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE671D1-3C26-4D28-ADCC-17123181BDE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA2F4A9-E2BE-4D3B-80A0-0D9483984E5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="140">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -454,7 +454,7 @@
     <t xml:space="preserve">GRANT SELECT on integracao.vw_bmh_online TO </t>
   </si>
   <si>
-    <t>flavia</t>
+    <t>irodrigues</t>
   </si>
 </sst>
 </file>
@@ -3700,7 +3700,7 @@
       </c>
       <c r="D59" t="str">
         <f>A59&amp;" "&amp;B59&amp;" "&amp;C59</f>
-        <v>CREATE USER  flavia PASSWORD '1234';</v>
+        <v>CREATE USER  irodrigues PASSWORD '1234';</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3715,7 +3715,7 @@
       </c>
       <c r="D60" t="str">
         <f t="shared" ref="D60:D126" si="0">A60&amp;" "&amp;B60&amp;" "&amp;C60</f>
-        <v>GRANT CONNECT ON DATABASE vila_verde TO  flavia ;</v>
+        <v>GRANT CONNECT ON DATABASE vila_verde TO  irodrigues ;</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3730,7 +3730,7 @@
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT USAGE ON SCHEMA integracao TO  flavia ;</v>
+        <v>GRANT USAGE ON SCHEMA integracao TO  irodrigues ;</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3745,7 +3745,7 @@
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  flavia ;</v>
+        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  irodrigues ;</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3760,7 +3760,7 @@
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  flavia ;</v>
+        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  irodrigues ;</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3775,7 +3775,7 @@
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO flavia ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO irodrigues ;</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  flavia ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  irodrigues ;</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="D66" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  flavia ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  irodrigues ;</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3820,7 +3820,7 @@
       </c>
       <c r="D67" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  flavia ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  irodrigues ;</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3835,7 +3835,7 @@
       </c>
       <c r="D68" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  flavia ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  irodrigues ;</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3850,7 +3850,7 @@
       </c>
       <c r="D69" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  flavia ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  irodrigues ;</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3865,7 +3865,7 @@
       </c>
       <c r="D70" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  flavia ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  irodrigues ;</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3880,7 +3880,7 @@
       </c>
       <c r="D71" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  flavia ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  irodrigues ;</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3895,7 +3895,7 @@
       </c>
       <c r="D72" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  flavia ;</v>
+        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  irodrigues ;</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3910,7 +3910,7 @@
       </c>
       <c r="D73" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to flavia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to irodrigues ;</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3925,7 +3925,7 @@
       </c>
       <c r="D74" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to flavia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to irodrigues ;</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3940,7 +3940,7 @@
       </c>
       <c r="D75" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to flavia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to irodrigues ;</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3955,7 +3955,7 @@
       </c>
       <c r="D76" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to flavia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to irodrigues ;</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3970,7 +3970,7 @@
       </c>
       <c r="D77" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to flavia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to irodrigues ;</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -3985,7 +3985,7 @@
       </c>
       <c r="D78" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to flavia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to irodrigues ;</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -4000,7 +4000,7 @@
       </c>
       <c r="D79" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to flavia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to irodrigues ;</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4015,7 +4015,7 @@
       </c>
       <c r="D80" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to flavia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to irodrigues ;</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -4030,7 +4030,7 @@
       </c>
       <c r="D81" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to flavia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to irodrigues ;</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4045,7 +4045,7 @@
       </c>
       <c r="D82" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO flavia ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO irodrigues ;</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -4060,7 +4060,7 @@
       </c>
       <c r="D83" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO flavia ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO irodrigues ;</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -4075,7 +4075,7 @@
       </c>
       <c r="D84" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  flavia ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  irodrigues ;</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -4090,7 +4090,7 @@
       </c>
       <c r="D85" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO flavia ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO irodrigues ;</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4105,7 +4105,7 @@
       </c>
       <c r="D86" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO flavia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO irodrigues ;</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4120,7 +4120,7 @@
       </c>
       <c r="D87" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO flavia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO irodrigues ;</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -4135,7 +4135,7 @@
       </c>
       <c r="D88" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO flavia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO irodrigues ;</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4150,7 +4150,7 @@
       </c>
       <c r="D89" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO flavia ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO irodrigues ;</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -4165,7 +4165,7 @@
       </c>
       <c r="D90" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  flavia ;</v>
+        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  irodrigues ;</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4180,7 +4180,7 @@
       </c>
       <c r="D91" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  flavia ;</v>
+        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  irodrigues ;</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4195,7 +4195,7 @@
       </c>
       <c r="D92" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_leito TO  flavia ;</v>
+        <v>GRANT SELECT on integracao.tb_leito TO  irodrigues ;</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -4210,7 +4210,7 @@
       </c>
       <c r="D93" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  flavia ;</v>
+        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  irodrigues ;</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4225,7 +4225,7 @@
       </c>
       <c r="D94" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_crtr_intnc TO  flavia ;</v>
+        <v>GRANT SELECT on integracao.tb_crtr_intnc TO  irodrigues ;</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -4240,7 +4240,7 @@
       </c>
       <c r="D95" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_dieta TO  flavia ;</v>
+        <v>GRANT SELECT on integracao.tb_dieta TO  irodrigues ;</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4255,7 +4255,22 @@
       </c>
       <c r="D96" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  flavia ;</v>
+        <v>GRANT SELECT on integracao.tb_const TO  irodrigues ;</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>138</v>
+      </c>
+      <c r="B97" t="s">
+        <v>139</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" ref="D97" si="1">A97&amp;" "&amp;B97&amp;" "&amp;C97</f>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  irodrigues ;</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4680,7 +4695,7 @@
         <v>1</v>
       </c>
       <c r="D127" t="str">
-        <f t="shared" ref="D127:D151" si="1">A127&amp;" "&amp;B127&amp;" "&amp;C127</f>
+        <f t="shared" ref="D127:D151" si="2">A127&amp;" "&amp;B127&amp;" "&amp;C127</f>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  bcorrea ;</v>
       </c>
     </row>
@@ -4695,7 +4710,7 @@
         <v>1</v>
       </c>
       <c r="D128" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  mmattos ;</v>
       </c>
     </row>
@@ -4710,7 +4725,7 @@
         <v>1</v>
       </c>
       <c r="D129" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  greis ;</v>
       </c>
     </row>
@@ -4725,7 +4740,7 @@
         <v>1</v>
       </c>
       <c r="D130" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  ldelgado ;</v>
       </c>
     </row>
@@ -4740,7 +4755,7 @@
         <v>1</v>
       </c>
       <c r="D131" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  deliza ;</v>
       </c>
     </row>
@@ -4755,7 +4770,7 @@
         <v>1</v>
       </c>
       <c r="D132" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  aalbino ;</v>
       </c>
     </row>
@@ -4770,7 +4785,7 @@
         <v>1</v>
       </c>
       <c r="D133" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  ralmeida ;</v>
       </c>
     </row>
@@ -4785,7 +4800,7 @@
         <v>1</v>
       </c>
       <c r="D134" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  bsouza ;</v>
       </c>
     </row>
@@ -4800,7 +4815,7 @@
         <v>1</v>
       </c>
       <c r="D135" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  tnovaes ;</v>
       </c>
     </row>
@@ -4815,7 +4830,7 @@
         <v>1</v>
       </c>
       <c r="D136" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  mliberato ;</v>
       </c>
     </row>
@@ -4830,7 +4845,7 @@
         <v>1</v>
       </c>
       <c r="D137" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  dchinelato ;</v>
       </c>
     </row>
@@ -4845,7 +4860,7 @@
         <v>1</v>
       </c>
       <c r="D138" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  amonteiro ;</v>
       </c>
     </row>
@@ -4860,7 +4875,7 @@
         <v>1</v>
       </c>
       <c r="D139" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  soliveira ;</v>
       </c>
     </row>
@@ -4875,7 +4890,7 @@
         <v>1</v>
       </c>
       <c r="D140" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  axavier ;</v>
       </c>
     </row>
@@ -4890,7 +4905,7 @@
         <v>1</v>
       </c>
       <c r="D141" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  opacheco ;</v>
       </c>
     </row>
@@ -4905,7 +4920,7 @@
         <v>1</v>
       </c>
       <c r="D142" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  fmedeiros ;</v>
       </c>
     </row>
@@ -4920,7 +4935,7 @@
         <v>1</v>
       </c>
       <c r="D143" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  sbhering ;</v>
       </c>
     </row>
@@ -4935,7 +4950,7 @@
         <v>1</v>
       </c>
       <c r="D144" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  vandrade ;</v>
       </c>
     </row>
@@ -4950,7 +4965,7 @@
         <v>1</v>
       </c>
       <c r="D145" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  dfajardo ;</v>
       </c>
     </row>
@@ -4965,7 +4980,7 @@
         <v>1</v>
       </c>
       <c r="D146" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  jmiguel ;</v>
       </c>
     </row>
@@ -4980,7 +4995,7 @@
         <v>1</v>
       </c>
       <c r="D147" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  coliveira ;</v>
       </c>
     </row>
@@ -4995,7 +5010,7 @@
         <v>1</v>
       </c>
       <c r="D148" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  pferreira ;</v>
       </c>
     </row>
@@ -5010,7 +5025,7 @@
         <v>1</v>
       </c>
       <c r="D149" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  amorais ;</v>
       </c>
     </row>
@@ -5025,7 +5040,7 @@
         <v>1</v>
       </c>
       <c r="D150" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  poliveira ;</v>
       </c>
     </row>
@@ -5040,7 +5055,7 @@
         <v>1</v>
       </c>
       <c r="D151" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>GRANT SELECT on integracao.vw_bmh_online TO  farmacia ;</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização do relatório por tipo
</commit_message>
<xml_diff>
--- a/script_base_dados/grants.xlsx
+++ b/script_base_dados/grants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\integracao\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA2F4A9-E2BE-4D3B-80A0-0D9483984E5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BBC6BA-683F-497A-B8C7-9C88D5616477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -454,14 +454,14 @@
     <t xml:space="preserve">GRANT SELECT on integracao.vw_bmh_online TO </t>
   </si>
   <si>
-    <t>irodrigues</t>
+    <t>afaria</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -482,6 +482,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -504,12 +510,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3692,7 +3701,7 @@
       <c r="A59" t="s">
         <v>78</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C59" t="s">
@@ -3700,14 +3709,14 @@
       </c>
       <c r="D59" t="str">
         <f>A59&amp;" "&amp;B59&amp;" "&amp;C59</f>
-        <v>CREATE USER  irodrigues PASSWORD '1234';</v>
+        <v>CREATE USER  afaria PASSWORD '1234';</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>88</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C60" t="s">
@@ -3715,14 +3724,14 @@
       </c>
       <c r="D60" t="str">
         <f t="shared" ref="D60:D126" si="0">A60&amp;" "&amp;B60&amp;" "&amp;C60</f>
-        <v>GRANT CONNECT ON DATABASE vila_verde TO  irodrigues ;</v>
+        <v>GRANT CONNECT ON DATABASE vila_verde TO  afaria ;</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>66</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C61" t="s">
@@ -3730,14 +3739,14 @@
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT USAGE ON SCHEMA integracao TO  irodrigues ;</v>
+        <v>GRANT USAGE ON SCHEMA integracao TO  afaria ;</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>67</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C62" t="s">
@@ -3745,14 +3754,14 @@
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  irodrigues ;</v>
+        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  afaria ;</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>68</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C63" t="s">
@@ -3760,14 +3769,14 @@
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  irodrigues ;</v>
+        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  afaria ;</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>69</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C64" t="s">
@@ -3775,14 +3784,14 @@
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO irodrigues ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO afaria ;</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>70</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C65" t="s">
@@ -3790,14 +3799,14 @@
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  irodrigues ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  afaria ;</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>71</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C66" t="s">
@@ -3805,14 +3814,14 @@
       </c>
       <c r="D66" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  irodrigues ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  afaria ;</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>72</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C67" t="s">
@@ -3820,14 +3829,14 @@
       </c>
       <c r="D67" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  irodrigues ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  afaria ;</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>73</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C68" t="s">
@@ -3835,14 +3844,14 @@
       </c>
       <c r="D68" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  irodrigues ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  afaria ;</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>74</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C69" t="s">
@@ -3850,14 +3859,14 @@
       </c>
       <c r="D69" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  irodrigues ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  afaria ;</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>75</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C70" t="s">
@@ -3865,14 +3874,14 @@
       </c>
       <c r="D70" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  irodrigues ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  afaria ;</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>76</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C71" t="s">
@@ -3880,14 +3889,14 @@
       </c>
       <c r="D71" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  irodrigues ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  afaria ;</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>77</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C72" t="s">
@@ -3895,14 +3904,14 @@
       </c>
       <c r="D72" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  irodrigues ;</v>
+        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  afaria ;</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>27</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C73" t="s">
@@ -3910,14 +3919,14 @@
       </c>
       <c r="D73" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to irodrigues ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to afaria ;</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>25</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C74" t="s">
@@ -3925,14 +3934,14 @@
       </c>
       <c r="D74" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to irodrigues ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to afaria ;</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>26</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C75" t="s">
@@ -3940,14 +3949,14 @@
       </c>
       <c r="D75" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to irodrigues ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to afaria ;</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>19</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C76" t="s">
@@ -3955,14 +3964,14 @@
       </c>
       <c r="D76" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to irodrigues ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to afaria ;</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>20</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C77" t="s">
@@ -3970,14 +3979,14 @@
       </c>
       <c r="D77" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to irodrigues ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to afaria ;</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>21</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C78" t="s">
@@ -3985,14 +3994,14 @@
       </c>
       <c r="D78" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to irodrigues ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to afaria ;</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>22</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C79" t="s">
@@ -4000,14 +4009,14 @@
       </c>
       <c r="D79" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to irodrigues ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to afaria ;</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>23</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C80" t="s">
@@ -4015,14 +4024,14 @@
       </c>
       <c r="D80" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to irodrigues ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to afaria ;</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>24</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C81" t="s">
@@ -4030,14 +4039,14 @@
       </c>
       <c r="D81" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to irodrigues ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to afaria ;</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>0</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C82" t="s">
@@ -4045,14 +4054,14 @@
       </c>
       <c r="D82" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO irodrigues ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO afaria ;</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>2</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C83" t="s">
@@ -4060,14 +4069,14 @@
       </c>
       <c r="D83" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO irodrigues ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO afaria ;</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>3</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C84" t="s">
@@ -4075,14 +4084,14 @@
       </c>
       <c r="D84" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  irodrigues ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  afaria ;</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>4</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C85" t="s">
@@ -4090,14 +4099,14 @@
       </c>
       <c r="D85" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO irodrigues ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO afaria ;</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>5</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C86" t="s">
@@ -4105,14 +4114,14 @@
       </c>
       <c r="D86" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO irodrigues ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO afaria ;</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>6</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C87" t="s">
@@ -4120,14 +4129,14 @@
       </c>
       <c r="D87" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO irodrigues ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO afaria ;</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>7</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C88" t="s">
@@ -4135,14 +4144,14 @@
       </c>
       <c r="D88" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO irodrigues ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO afaria ;</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>8</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C89" t="s">
@@ -4150,14 +4159,14 @@
       </c>
       <c r="D89" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO irodrigues ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO afaria ;</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>86</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C90" t="s">
@@ -4165,14 +4174,14 @@
       </c>
       <c r="D90" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  irodrigues ;</v>
+        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  afaria ;</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>87</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C91" t="s">
@@ -4180,14 +4189,14 @@
       </c>
       <c r="D91" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  irodrigues ;</v>
+        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  afaria ;</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>84</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C92" t="s">
@@ -4195,14 +4204,14 @@
       </c>
       <c r="D92" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_leito TO  irodrigues ;</v>
+        <v>GRANT SELECT on integracao.tb_leito TO  afaria ;</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>85</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C93" t="s">
@@ -4210,14 +4219,14 @@
       </c>
       <c r="D93" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  irodrigues ;</v>
+        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  afaria ;</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>111</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C94" t="s">
@@ -4225,14 +4234,14 @@
       </c>
       <c r="D94" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_crtr_intnc TO  irodrigues ;</v>
+        <v>GRANT SELECT on integracao.tb_crtr_intnc TO  afaria ;</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>112</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C95" t="s">
@@ -4240,14 +4249,14 @@
       </c>
       <c r="D95" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_dieta TO  irodrigues ;</v>
+        <v>GRANT SELECT on integracao.tb_dieta TO  afaria ;</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>114</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C96" t="s">
@@ -4255,14 +4264,14 @@
       </c>
       <c r="D96" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  irodrigues ;</v>
+        <v>GRANT SELECT on integracao.tb_const TO  afaria ;</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>138</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="3" t="s">
         <v>139</v>
       </c>
       <c r="C97" t="s">
@@ -4270,7 +4279,7 @@
       </c>
       <c r="D97" t="str">
         <f t="shared" ref="D97" si="1">A97&amp;" "&amp;B97&amp;" "&amp;C97</f>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  irodrigues ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  afaria ;</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Criação do cadastro de transação
</commit_message>
<xml_diff>
--- a/script_base_dados/grants.xlsx
+++ b/script_base_dados/grants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\integracao\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0C0184-D883-458A-8DF1-5EBA3DA55D87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C102B6C-AA8E-4D01-A676-6AD0717CC08F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="141">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -455,6 +455,9 @@
   </si>
   <si>
     <t>jbarros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO </t>
   </si>
 </sst>
 </file>
@@ -3302,7 +3305,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
   <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100:D151"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4290,7 +4295,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B100" t="s">
         <v>44</v>
@@ -4300,12 +4305,12 @@
       </c>
       <c r="D100" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  aoliveira ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  aoliveira ;</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B101" t="s">
         <v>45</v>
@@ -4315,12 +4320,12 @@
       </c>
       <c r="D101" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  dalves ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  dalves ;</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B102" t="s">
         <v>46</v>
@@ -4330,12 +4335,12 @@
       </c>
       <c r="D102" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  emenezes ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  emenezes ;</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B103" t="s">
         <v>47</v>
@@ -4345,12 +4350,12 @@
       </c>
       <c r="D103" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  gcassia ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  gcassia ;</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B104" t="s">
         <v>48</v>
@@ -4360,12 +4365,12 @@
       </c>
       <c r="D104" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  lmaria ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  lmaria ;</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B105" t="s">
         <v>53</v>
@@ -4375,12 +4380,12 @@
       </c>
       <c r="D105" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  mrezende ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  mrezende ;</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B106" t="s">
         <v>49</v>
@@ -4390,12 +4395,12 @@
       </c>
       <c r="D106" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  lvieira ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  lvieira ;</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B107" t="s">
         <v>54</v>
@@ -4405,12 +4410,12 @@
       </c>
       <c r="D107" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  tsilva ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  tsilva ;</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B108" t="s">
         <v>50</v>
@@ -4420,12 +4425,12 @@
       </c>
       <c r="D108" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  vrodrigues ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  vrodrigues ;</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B109" t="s">
         <v>51</v>
@@ -4435,12 +4440,12 @@
       </c>
       <c r="D109" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  vlucia ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  vlucia ;</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B110" t="s">
         <v>55</v>
@@ -4450,12 +4455,12 @@
       </c>
       <c r="D110" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  vsilva ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  vsilva ;</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B111" t="s">
         <v>56</v>
@@ -4465,12 +4470,12 @@
       </c>
       <c r="D111" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  woliveira ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  woliveira ;</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B112" t="s">
         <v>52</v>
@@ -4480,12 +4485,12 @@
       </c>
       <c r="D112" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  wquetz ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  wquetz ;</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B113" t="s">
         <v>30</v>
@@ -4495,12 +4500,12 @@
       </c>
       <c r="D113" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  ftesta ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  ftesta ;</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B114" t="s">
         <v>59</v>
@@ -4510,12 +4515,12 @@
       </c>
       <c r="D114" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  simone ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  simone ;</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B115" t="s">
         <v>61</v>
@@ -4525,12 +4530,12 @@
       </c>
       <c r="D115" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  grazielle ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  grazielle ;</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B116" t="s">
         <v>63</v>
@@ -4540,12 +4545,12 @@
       </c>
       <c r="D116" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  dayane ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  dayane ;</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B117" t="s">
         <v>65</v>
@@ -4555,12 +4560,12 @@
       </c>
       <c r="D117" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  ronan ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  ronan ;</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B118" t="s">
         <v>10</v>
@@ -4570,12 +4575,12 @@
       </c>
       <c r="D118" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  clovismelo ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  clovismelo ;</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B119" t="s">
         <v>11</v>
@@ -4585,12 +4590,12 @@
       </c>
       <c r="D119" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  mariabethania ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  mariabethania ;</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B120" t="s">
         <v>12</v>
@@ -4600,12 +4605,12 @@
       </c>
       <c r="D120" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  fernandazeferino ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  fernandazeferino ;</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B121" t="s">
         <v>81</v>
@@ -4615,12 +4620,12 @@
       </c>
       <c r="D121" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  camila ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  camila ;</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B122" t="s">
         <v>113</v>
@@ -4630,12 +4635,12 @@
       </c>
       <c r="D122" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  administrativo ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  administrativo ;</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B123" t="s">
         <v>83</v>
@@ -4645,12 +4650,12 @@
       </c>
       <c r="D123" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  tivilaverde ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  tivilaverde ;</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B124" t="s">
         <v>16</v>
@@ -4660,12 +4665,12 @@
       </c>
       <c r="D124" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  lamorim ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  lamorim ;</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B125" t="s">
         <v>13</v>
@@ -4675,12 +4680,12 @@
       </c>
       <c r="D125" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  mvilela ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  mvilela ;</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B126" t="s">
         <v>14</v>
@@ -4690,12 +4695,12 @@
       </c>
       <c r="D126" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  fcampos ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  fcampos ;</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B127" t="s">
         <v>15</v>
@@ -4705,12 +4710,12 @@
       </c>
       <c r="D127" t="str">
         <f t="shared" ref="D127:D151" si="2">A127&amp;" "&amp;B127&amp;" "&amp;C127</f>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  bcorrea ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  bcorrea ;</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B128" t="s">
         <v>9</v>
@@ -4720,12 +4725,12 @@
       </c>
       <c r="D128" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  mmattos ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  mmattos ;</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B129" t="s">
         <v>92</v>
@@ -4735,12 +4740,12 @@
       </c>
       <c r="D129" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  greis ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  greis ;</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B130" t="s">
         <v>93</v>
@@ -4750,12 +4755,12 @@
       </c>
       <c r="D130" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  ldelgado ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  ldelgado ;</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B131" t="s">
         <v>94</v>
@@ -4765,12 +4770,12 @@
       </c>
       <c r="D131" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  deliza ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  deliza ;</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B132" t="s">
         <v>102</v>
@@ -4780,12 +4785,12 @@
       </c>
       <c r="D132" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  aalbino ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  aalbino ;</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B133" t="s">
         <v>103</v>
@@ -4795,12 +4800,12 @@
       </c>
       <c r="D133" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  ralmeida ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  ralmeida ;</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B134" t="s">
         <v>104</v>
@@ -4810,12 +4815,12 @@
       </c>
       <c r="D134" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  bsouza ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  bsouza ;</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B135" t="s">
         <v>105</v>
@@ -4825,12 +4830,12 @@
       </c>
       <c r="D135" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  tnovaes ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  tnovaes ;</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B136" t="s">
         <v>106</v>
@@ -4840,12 +4845,12 @@
       </c>
       <c r="D136" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  mliberato ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  mliberato ;</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B137" t="s">
         <v>107</v>
@@ -4855,12 +4860,12 @@
       </c>
       <c r="D137" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  dchinelato ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  dchinelato ;</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B138" t="s">
         <v>108</v>
@@ -4870,12 +4875,12 @@
       </c>
       <c r="D138" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  amonteiro ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  amonteiro ;</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B139" t="s">
         <v>110</v>
@@ -4885,12 +4890,12 @@
       </c>
       <c r="D139" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  soliveira ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  soliveira ;</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B140" t="s">
         <v>126</v>
@@ -4900,12 +4905,12 @@
       </c>
       <c r="D140" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  axavier ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  axavier ;</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B141" t="s">
         <v>127</v>
@@ -4915,12 +4920,12 @@
       </c>
       <c r="D141" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  opacheco ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  opacheco ;</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B142" t="s">
         <v>128</v>
@@ -4930,12 +4935,12 @@
       </c>
       <c r="D142" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  fmedeiros ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  fmedeiros ;</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B143" t="s">
         <v>130</v>
@@ -4945,12 +4950,12 @@
       </c>
       <c r="D143" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  sbhering ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  sbhering ;</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B144" t="s">
         <v>131</v>
@@ -4960,12 +4965,12 @@
       </c>
       <c r="D144" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  vandrade ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  vandrade ;</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B145" t="s">
         <v>129</v>
@@ -4975,12 +4980,12 @@
       </c>
       <c r="D145" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  dfajardo ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  dfajardo ;</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B146" t="s">
         <v>132</v>
@@ -4990,12 +4995,12 @@
       </c>
       <c r="D146" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  jmiguel ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  jmiguel ;</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B147" t="s">
         <v>133</v>
@@ -5005,12 +5010,12 @@
       </c>
       <c r="D147" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  coliveira ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  coliveira ;</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B148" t="s">
         <v>134</v>
@@ -5020,12 +5025,12 @@
       </c>
       <c r="D148" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  pferreira ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  pferreira ;</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B149" t="s">
         <v>135</v>
@@ -5035,12 +5040,12 @@
       </c>
       <c r="D149" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  amorais ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  amorais ;</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B150" t="s">
         <v>136</v>
@@ -5050,12 +5055,12 @@
       </c>
       <c r="D150" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  poliveira ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  poliveira ;</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B151" t="s">
         <v>137</v>
@@ -5065,7 +5070,7 @@
       </c>
       <c r="D151" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  farmacia ;</v>
+        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  farmacia ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de status do leito
</commit_message>
<xml_diff>
--- a/script_base_dados/grants.xlsx
+++ b/script_base_dados/grants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\integracao\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C102B6C-AA8E-4D01-A676-6AD0717CC08F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AE0DB3-9EC1-4FA2-AAD8-68C9D542E39E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -457,7 +457,7 @@
     <t>jbarros</t>
   </si>
   <si>
-    <t xml:space="preserve">GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO </t>
+    <t>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO</t>
   </si>
 </sst>
 </file>
@@ -3305,7 +3305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
   <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
       <selection activeCell="D100" sqref="D100:D151"/>
     </sheetView>
   </sheetViews>
@@ -4305,7 +4305,7 @@
       </c>
       <c r="D100" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  aoliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO aoliveira ;</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4320,7 +4320,7 @@
       </c>
       <c r="D101" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  dalves ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO dalves ;</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4335,7 +4335,7 @@
       </c>
       <c r="D102" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  emenezes ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO emenezes ;</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4350,7 +4350,7 @@
       </c>
       <c r="D103" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  gcassia ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO gcassia ;</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4365,7 +4365,7 @@
       </c>
       <c r="D104" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  lmaria ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO lmaria ;</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4380,7 +4380,7 @@
       </c>
       <c r="D105" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  mrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO mrezende ;</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4395,7 +4395,7 @@
       </c>
       <c r="D106" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  lvieira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO lvieira ;</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4410,7 +4410,7 @@
       </c>
       <c r="D107" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  tsilva ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO tsilva ;</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4425,7 +4425,7 @@
       </c>
       <c r="D108" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  vrodrigues ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO vrodrigues ;</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4440,7 +4440,7 @@
       </c>
       <c r="D109" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  vlucia ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO vlucia ;</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4455,7 +4455,7 @@
       </c>
       <c r="D110" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  vsilva ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO vsilva ;</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4470,7 +4470,7 @@
       </c>
       <c r="D111" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  woliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO woliveira ;</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4485,7 +4485,7 @@
       </c>
       <c r="D112" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  wquetz ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO wquetz ;</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -4500,7 +4500,7 @@
       </c>
       <c r="D113" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  ftesta ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO ftesta ;</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -4515,7 +4515,7 @@
       </c>
       <c r="D114" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  simone ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO simone ;</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -4530,7 +4530,7 @@
       </c>
       <c r="D115" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  grazielle ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO grazielle ;</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -4545,7 +4545,7 @@
       </c>
       <c r="D116" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  dayane ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO dayane ;</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -4560,7 +4560,7 @@
       </c>
       <c r="D117" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  ronan ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO ronan ;</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -4575,7 +4575,7 @@
       </c>
       <c r="D118" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  clovismelo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO clovismelo ;</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -4590,7 +4590,7 @@
       </c>
       <c r="D119" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  mariabethania ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO mariabethania ;</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -4605,7 +4605,7 @@
       </c>
       <c r="D120" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  fernandazeferino ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO fernandazeferino ;</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -4620,7 +4620,7 @@
       </c>
       <c r="D121" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  camila ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO camila ;</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -4635,7 +4635,7 @@
       </c>
       <c r="D122" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  administrativo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO administrativo ;</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -4650,7 +4650,7 @@
       </c>
       <c r="D123" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  tivilaverde ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO tivilaverde ;</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -4665,7 +4665,7 @@
       </c>
       <c r="D124" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  lamorim ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO lamorim ;</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -4680,7 +4680,7 @@
       </c>
       <c r="D125" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  mvilela ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO mvilela ;</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -4695,7 +4695,7 @@
       </c>
       <c r="D126" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  fcampos ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO fcampos ;</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -4710,7 +4710,7 @@
       </c>
       <c r="D127" t="str">
         <f t="shared" ref="D127:D151" si="2">A127&amp;" "&amp;B127&amp;" "&amp;C127</f>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  bcorrea ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO bcorrea ;</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="D128" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  mmattos ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO mmattos ;</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -4740,7 +4740,7 @@
       </c>
       <c r="D129" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  greis ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO greis ;</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -4755,7 +4755,7 @@
       </c>
       <c r="D130" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  ldelgado ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO ldelgado ;</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -4770,7 +4770,7 @@
       </c>
       <c r="D131" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  deliza ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO deliza ;</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -4785,7 +4785,7 @@
       </c>
       <c r="D132" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  aalbino ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO aalbino ;</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -4800,7 +4800,7 @@
       </c>
       <c r="D133" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  ralmeida ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO ralmeida ;</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -4815,7 +4815,7 @@
       </c>
       <c r="D134" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  bsouza ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO bsouza ;</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -4830,7 +4830,7 @@
       </c>
       <c r="D135" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  tnovaes ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO tnovaes ;</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -4845,7 +4845,7 @@
       </c>
       <c r="D136" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  mliberato ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO mliberato ;</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -4860,7 +4860,7 @@
       </c>
       <c r="D137" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  dchinelato ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO dchinelato ;</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -4875,7 +4875,7 @@
       </c>
       <c r="D138" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  amonteiro ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO amonteiro ;</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -4890,7 +4890,7 @@
       </c>
       <c r="D139" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  soliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO soliveira ;</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -4905,7 +4905,7 @@
       </c>
       <c r="D140" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  axavier ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO axavier ;</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -4920,7 +4920,7 @@
       </c>
       <c r="D141" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  opacheco ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO opacheco ;</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -4935,7 +4935,7 @@
       </c>
       <c r="D142" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  fmedeiros ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO fmedeiros ;</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -4950,7 +4950,7 @@
       </c>
       <c r="D143" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  sbhering ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO sbhering ;</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -4965,7 +4965,7 @@
       </c>
       <c r="D144" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  vandrade ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO vandrade ;</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -4980,7 +4980,7 @@
       </c>
       <c r="D145" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  dfajardo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO dfajardo ;</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -4995,7 +4995,7 @@
       </c>
       <c r="D146" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  jmiguel ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO jmiguel ;</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -5010,7 +5010,7 @@
       </c>
       <c r="D147" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  coliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO coliveira ;</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -5025,7 +5025,7 @@
       </c>
       <c r="D148" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  pferreira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO pferreira ;</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -5040,7 +5040,7 @@
       </c>
       <c r="D149" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  amorais ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO amorais ;</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -5055,7 +5055,7 @@
       </c>
       <c r="D150" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  poliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO poliveira ;</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -5070,7 +5070,7 @@
       </c>
       <c r="D151" t="str">
         <f t="shared" si="2"/>
-        <v>GRANT SELECT on integracao.tb_c_acesso_transac_integracao TO  farmacia ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO farmacia ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Melhoria no arquivo de grants.xlsx
</commit_message>
<xml_diff>
--- a/script_base_dados/grants.xlsx
+++ b/script_base_dados/grants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\integracao\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AE0DB3-9EC1-4FA2-AAD8-68C9D542E39E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A4502B-741D-4C57-BBE5-EB87A615B1BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="154">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -376,9 +376,6 @@
     <t xml:space="preserve">GRANT SELECT on integracao.tb_dieta TO </t>
   </si>
   <si>
-    <t>administrativo</t>
-  </si>
-  <si>
     <t xml:space="preserve">GRANT SELECT on integracao.tb_const TO </t>
   </si>
   <si>
@@ -454,10 +451,52 @@
     <t xml:space="preserve">GRANT SELECT on integracao.vw_bmh_online TO </t>
   </si>
   <si>
-    <t>jbarros</t>
-  </si>
-  <si>
-    <t>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO</t>
+    <t>GRANT ALL ON SEQUENCE integracao.sq_acesso_transac_integracao to</t>
+  </si>
+  <si>
+    <t>GRANT ALL ON SEQUENCE integracao.sq_equip_hosptr to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT ALL ON SEQUENCE integracao.sq_grupo_acesso to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_acesso to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_menu_sist_integracao to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_transac_acesso to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT ALL ON SEQUENCE integracao.sq_grvd_risco_pcnt to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT ALL ON SEQUENCE integracao.sq_log_acesso to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT ALL ON SEQUENCE integracao.sq_menu_sist_integracao to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT ALL ON SEQUENCE integracao.sq_mtvo_alta to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT ALL ON SEQUENCE integracao.sq_orig_dmnd_plnj_leito to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT ALL ON SEQUENCE integracao.sq_plnj_pcnt_leito to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT ALL ON SEQUENCE integracao.sq_status_leito to </t>
+  </si>
+  <si>
+    <t>GRANT ALL ON SEQUENCE integracao.sq_usua_acesso to</t>
+  </si>
+  <si>
+    <t>lrezende</t>
   </si>
 </sst>
 </file>
@@ -3303,10 +3342,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
-  <dimension ref="A1:D151"/>
+  <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100:D151"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59:D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3611,95 +3650,95 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B46" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B47" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B49" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B50" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B53" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B55" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B56" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3707,14 +3746,14 @@
         <v>78</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C59" t="s">
         <v>79</v>
       </c>
       <c r="D59" t="str">
         <f>A59&amp;" "&amp;B59&amp;" "&amp;C59</f>
-        <v>CREATE USER  jbarros PASSWORD '1234';</v>
+        <v>CREATE USER  lrezende PASSWORD '1234';</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3722,14 +3761,14 @@
         <v>88</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C60" t="s">
         <v>1</v>
       </c>
       <c r="D60" t="str">
-        <f t="shared" ref="D60:D126" si="0">A60&amp;" "&amp;B60&amp;" "&amp;C60</f>
-        <v>GRANT CONNECT ON DATABASE vila_verde TO  jbarros ;</v>
+        <f t="shared" ref="D60:D112" si="0">A60&amp;" "&amp;B60&amp;" "&amp;C60</f>
+        <v>GRANT CONNECT ON DATABASE vila_verde TO  lrezende ;</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3737,14 +3776,14 @@
         <v>66</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C61" t="s">
         <v>1</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT USAGE ON SCHEMA integracao TO  jbarros ;</v>
+        <v>GRANT USAGE ON SCHEMA integracao TO  lrezende ;</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3752,14 +3791,14 @@
         <v>67</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C62" t="s">
         <v>1</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  jbarros ;</v>
+        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  lrezende ;</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3767,14 +3806,14 @@
         <v>68</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C63" t="s">
         <v>1</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  jbarros ;</v>
+        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  lrezende ;</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3782,14 +3821,14 @@
         <v>69</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C64" t="s">
         <v>1</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO jbarros ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO lrezende ;</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3797,14 +3836,14 @@
         <v>70</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C65" t="s">
         <v>1</v>
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  jbarros ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  lrezende ;</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3812,14 +3851,14 @@
         <v>71</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C66" t="s">
         <v>1</v>
       </c>
       <c r="D66" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  jbarros ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  lrezende ;</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3827,14 +3866,14 @@
         <v>72</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C67" t="s">
         <v>1</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  jbarros ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  lrezende ;</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3842,14 +3881,14 @@
         <v>73</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C68" t="s">
         <v>1</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  jbarros ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  lrezende ;</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3857,14 +3896,14 @@
         <v>74</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C69" t="s">
         <v>1</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  jbarros ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  lrezende ;</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3872,14 +3911,14 @@
         <v>75</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C70" t="s">
         <v>1</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  jbarros ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  lrezende ;</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3887,14 +3926,14 @@
         <v>76</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C71" t="s">
         <v>1</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  jbarros ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  lrezende ;</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3902,14 +3941,14 @@
         <v>77</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C72" t="s">
         <v>1</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  jbarros ;</v>
+        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  lrezende ;</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3917,14 +3956,14 @@
         <v>27</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C73" t="s">
         <v>1</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to jbarros ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to lrezende ;</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3932,14 +3971,14 @@
         <v>25</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C74" t="s">
         <v>1</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to jbarros ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to lrezende ;</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3947,14 +3986,14 @@
         <v>26</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C75" t="s">
         <v>1</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to jbarros ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to lrezende ;</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3962,14 +4001,14 @@
         <v>19</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C76" t="s">
         <v>1</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to jbarros ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to lrezende ;</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3977,14 +4016,14 @@
         <v>20</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to jbarros ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to lrezende ;</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -3992,14 +4031,14 @@
         <v>21</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C78" t="s">
         <v>1</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to jbarros ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to lrezende ;</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -4007,14 +4046,14 @@
         <v>22</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C79" t="s">
         <v>1</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to jbarros ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to lrezende ;</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4022,14 +4061,14 @@
         <v>23</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C80" t="s">
         <v>1</v>
       </c>
       <c r="D80" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to jbarros ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to lrezende ;</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -4037,14 +4076,14 @@
         <v>24</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C81" t="s">
         <v>1</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to jbarros ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to lrezende ;</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4052,14 +4091,14 @@
         <v>0</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C82" t="s">
         <v>1</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO jbarros ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO lrezende ;</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -4067,14 +4106,14 @@
         <v>2</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C83" t="s">
         <v>1</v>
       </c>
       <c r="D83" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO jbarros ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO lrezende ;</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -4082,14 +4121,14 @@
         <v>3</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C84" t="s">
         <v>1</v>
       </c>
       <c r="D84" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  jbarros ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  lrezende ;</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -4097,14 +4136,14 @@
         <v>4</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C85" t="s">
         <v>1</v>
       </c>
       <c r="D85" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO jbarros ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO lrezende ;</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4112,14 +4151,14 @@
         <v>5</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C86" t="s">
         <v>1</v>
       </c>
       <c r="D86" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO jbarros ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO lrezende ;</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4127,14 +4166,14 @@
         <v>6</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C87" t="s">
         <v>1</v>
       </c>
       <c r="D87" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO jbarros ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO lrezende ;</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -4142,14 +4181,14 @@
         <v>7</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C88" t="s">
         <v>1</v>
       </c>
       <c r="D88" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO jbarros ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO lrezende ;</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4157,14 +4196,14 @@
         <v>8</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C89" t="s">
         <v>1</v>
       </c>
       <c r="D89" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO jbarros ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO lrezende ;</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -4172,14 +4211,14 @@
         <v>86</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C90" t="s">
         <v>1</v>
       </c>
       <c r="D90" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  jbarros ;</v>
+        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  lrezende ;</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4187,14 +4226,14 @@
         <v>87</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C91" t="s">
         <v>1</v>
       </c>
       <c r="D91" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  jbarros ;</v>
+        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  lrezende ;</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4202,14 +4241,14 @@
         <v>84</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C92" t="s">
         <v>1</v>
       </c>
       <c r="D92" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_leito TO  jbarros ;</v>
+        <v>GRANT SELECT on integracao.tb_leito TO  lrezende ;</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -4217,14 +4256,14 @@
         <v>85</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C93" t="s">
         <v>1</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  jbarros ;</v>
+        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  lrezende ;</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4232,14 +4271,14 @@
         <v>111</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C94" t="s">
         <v>1</v>
       </c>
       <c r="D94" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_crtr_intnc TO  jbarros ;</v>
+        <v>GRANT SELECT on integracao.tb_crtr_intnc TO  lrezende ;</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -4247,830 +4286,269 @@
         <v>112</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C95" t="s">
         <v>1</v>
       </c>
       <c r="D95" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_dieta TO  jbarros ;</v>
+        <v>GRANT SELECT on integracao.tb_dieta TO  lrezende ;</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C96" t="s">
         <v>1</v>
       </c>
       <c r="D96" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  jbarros ;</v>
+        <v>GRANT SELECT on integracao.tb_const TO  lrezende ;</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C97" t="s">
         <v>1</v>
       </c>
       <c r="D97" t="str">
         <f t="shared" ref="D97" si="1">A97&amp;" "&amp;B97&amp;" "&amp;C97</f>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  jbarros ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  lrezende ;</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>138</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_acesso_transac_integracao to lrezende ;</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>139</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1</v>
+      </c>
       <c r="D99" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_equip_hosptr to lrezende ;</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>140</v>
       </c>
-      <c r="B100" t="s">
-        <v>44</v>
+      <c r="B100" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C100" t="s">
         <v>1</v>
       </c>
       <c r="D100" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO aoliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_acesso to  lrezende ;</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>140</v>
-      </c>
-      <c r="B101" t="s">
-        <v>45</v>
+        <v>141</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C101" t="s">
         <v>1</v>
       </c>
       <c r="D101" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO dalves ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_acesso to  lrezende ;</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>140</v>
-      </c>
-      <c r="B102" t="s">
-        <v>46</v>
+        <v>142</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C102" t="s">
         <v>1</v>
       </c>
       <c r="D102" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO emenezes ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_menu_sist_integracao to  lrezende ;</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>140</v>
-      </c>
-      <c r="B103" t="s">
-        <v>47</v>
+        <v>143</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C103" t="s">
         <v>1</v>
       </c>
       <c r="D103" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO gcassia ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_transac_acesso to  lrezende ;</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>140</v>
-      </c>
-      <c r="B104" t="s">
-        <v>48</v>
+        <v>144</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C104" t="s">
         <v>1</v>
       </c>
       <c r="D104" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO lmaria ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grvd_risco_pcnt to  lrezende ;</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>140</v>
-      </c>
-      <c r="B105" t="s">
-        <v>53</v>
+        <v>145</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C105" t="s">
         <v>1</v>
       </c>
       <c r="D105" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO mrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status to  lrezende ;</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>140</v>
-      </c>
-      <c r="B106" t="s">
-        <v>49</v>
+        <v>146</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C106" t="s">
         <v>1</v>
       </c>
       <c r="D106" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO lvieira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso to  lrezende ;</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>140</v>
-      </c>
-      <c r="B107" t="s">
-        <v>54</v>
+        <v>147</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C107" t="s">
         <v>1</v>
       </c>
       <c r="D107" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO tsilva ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_menu_sist_integracao to  lrezende ;</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>140</v>
-      </c>
-      <c r="B108" t="s">
-        <v>50</v>
+        <v>148</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C108" t="s">
         <v>1</v>
       </c>
       <c r="D108" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO vrodrigues ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_mtvo_alta to  lrezende ;</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>140</v>
-      </c>
-      <c r="B109" t="s">
-        <v>51</v>
+        <v>149</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C109" t="s">
         <v>1</v>
       </c>
       <c r="D109" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO vlucia ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_orig_dmnd_plnj_leito to  lrezende ;</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>140</v>
-      </c>
-      <c r="B110" t="s">
-        <v>55</v>
+        <v>150</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C110" t="s">
         <v>1</v>
       </c>
       <c r="D110" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO vsilva ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_plnj_pcnt_leito to  lrezende ;</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>140</v>
-      </c>
-      <c r="B111" t="s">
-        <v>56</v>
+        <v>151</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C111" t="s">
         <v>1</v>
       </c>
       <c r="D111" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO woliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_status_leito to  lrezende ;</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>140</v>
-      </c>
-      <c r="B112" t="s">
-        <v>52</v>
+        <v>152</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C112" t="s">
         <v>1</v>
       </c>
       <c r="D112" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO wquetz ;</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>140</v>
-      </c>
-      <c r="B113" t="s">
-        <v>30</v>
-      </c>
-      <c r="C113" t="s">
-        <v>1</v>
-      </c>
-      <c r="D113" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO ftesta ;</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>140</v>
-      </c>
-      <c r="B114" t="s">
-        <v>59</v>
-      </c>
-      <c r="C114" t="s">
-        <v>1</v>
-      </c>
-      <c r="D114" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO simone ;</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>140</v>
-      </c>
-      <c r="B115" t="s">
-        <v>61</v>
-      </c>
-      <c r="C115" t="s">
-        <v>1</v>
-      </c>
-      <c r="D115" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO grazielle ;</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>140</v>
-      </c>
-      <c r="B116" t="s">
-        <v>63</v>
-      </c>
-      <c r="C116" t="s">
-        <v>1</v>
-      </c>
-      <c r="D116" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO dayane ;</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>140</v>
-      </c>
-      <c r="B117" t="s">
-        <v>65</v>
-      </c>
-      <c r="C117" t="s">
-        <v>1</v>
-      </c>
-      <c r="D117" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO ronan ;</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>140</v>
-      </c>
-      <c r="B118" t="s">
-        <v>10</v>
-      </c>
-      <c r="C118" t="s">
-        <v>1</v>
-      </c>
-      <c r="D118" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO clovismelo ;</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>140</v>
-      </c>
-      <c r="B119" t="s">
-        <v>11</v>
-      </c>
-      <c r="C119" t="s">
-        <v>1</v>
-      </c>
-      <c r="D119" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO mariabethania ;</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>140</v>
-      </c>
-      <c r="B120" t="s">
-        <v>12</v>
-      </c>
-      <c r="C120" t="s">
-        <v>1</v>
-      </c>
-      <c r="D120" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO fernandazeferino ;</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>140</v>
-      </c>
-      <c r="B121" t="s">
-        <v>81</v>
-      </c>
-      <c r="C121" t="s">
-        <v>1</v>
-      </c>
-      <c r="D121" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO camila ;</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>140</v>
-      </c>
-      <c r="B122" t="s">
-        <v>113</v>
-      </c>
-      <c r="C122" t="s">
-        <v>1</v>
-      </c>
-      <c r="D122" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO administrativo ;</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>140</v>
-      </c>
-      <c r="B123" t="s">
-        <v>83</v>
-      </c>
-      <c r="C123" t="s">
-        <v>1</v>
-      </c>
-      <c r="D123" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO tivilaverde ;</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>140</v>
-      </c>
-      <c r="B124" t="s">
-        <v>16</v>
-      </c>
-      <c r="C124" t="s">
-        <v>1</v>
-      </c>
-      <c r="D124" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO lamorim ;</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>140</v>
-      </c>
-      <c r="B125" t="s">
-        <v>13</v>
-      </c>
-      <c r="C125" t="s">
-        <v>1</v>
-      </c>
-      <c r="D125" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO mvilela ;</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>140</v>
-      </c>
-      <c r="B126" t="s">
-        <v>14</v>
-      </c>
-      <c r="C126" t="s">
-        <v>1</v>
-      </c>
-      <c r="D126" t="str">
-        <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO fcampos ;</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>140</v>
-      </c>
-      <c r="B127" t="s">
-        <v>15</v>
-      </c>
-      <c r="C127" t="s">
-        <v>1</v>
-      </c>
-      <c r="D127" t="str">
-        <f t="shared" ref="D127:D151" si="2">A127&amp;" "&amp;B127&amp;" "&amp;C127</f>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO bcorrea ;</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>140</v>
-      </c>
-      <c r="B128" t="s">
-        <v>9</v>
-      </c>
-      <c r="C128" t="s">
-        <v>1</v>
-      </c>
-      <c r="D128" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO mmattos ;</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>140</v>
-      </c>
-      <c r="B129" t="s">
-        <v>92</v>
-      </c>
-      <c r="C129" t="s">
-        <v>1</v>
-      </c>
-      <c r="D129" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO greis ;</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>140</v>
-      </c>
-      <c r="B130" t="s">
-        <v>93</v>
-      </c>
-      <c r="C130" t="s">
-        <v>1</v>
-      </c>
-      <c r="D130" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO ldelgado ;</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>140</v>
-      </c>
-      <c r="B131" t="s">
-        <v>94</v>
-      </c>
-      <c r="C131" t="s">
-        <v>1</v>
-      </c>
-      <c r="D131" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO deliza ;</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>140</v>
-      </c>
-      <c r="B132" t="s">
-        <v>102</v>
-      </c>
-      <c r="C132" t="s">
-        <v>1</v>
-      </c>
-      <c r="D132" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO aalbino ;</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>140</v>
-      </c>
-      <c r="B133" t="s">
-        <v>103</v>
-      </c>
-      <c r="C133" t="s">
-        <v>1</v>
-      </c>
-      <c r="D133" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO ralmeida ;</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>140</v>
-      </c>
-      <c r="B134" t="s">
-        <v>104</v>
-      </c>
-      <c r="C134" t="s">
-        <v>1</v>
-      </c>
-      <c r="D134" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO bsouza ;</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>140</v>
-      </c>
-      <c r="B135" t="s">
-        <v>105</v>
-      </c>
-      <c r="C135" t="s">
-        <v>1</v>
-      </c>
-      <c r="D135" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO tnovaes ;</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>140</v>
-      </c>
-      <c r="B136" t="s">
-        <v>106</v>
-      </c>
-      <c r="C136" t="s">
-        <v>1</v>
-      </c>
-      <c r="D136" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO mliberato ;</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>140</v>
-      </c>
-      <c r="B137" t="s">
-        <v>107</v>
-      </c>
-      <c r="C137" t="s">
-        <v>1</v>
-      </c>
-      <c r="D137" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO dchinelato ;</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>140</v>
-      </c>
-      <c r="B138" t="s">
-        <v>108</v>
-      </c>
-      <c r="C138" t="s">
-        <v>1</v>
-      </c>
-      <c r="D138" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO amonteiro ;</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>140</v>
-      </c>
-      <c r="B139" t="s">
-        <v>110</v>
-      </c>
-      <c r="C139" t="s">
-        <v>1</v>
-      </c>
-      <c r="D139" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO soliveira ;</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>140</v>
-      </c>
-      <c r="B140" t="s">
-        <v>126</v>
-      </c>
-      <c r="C140" t="s">
-        <v>1</v>
-      </c>
-      <c r="D140" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO axavier ;</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>140</v>
-      </c>
-      <c r="B141" t="s">
-        <v>127</v>
-      </c>
-      <c r="C141" t="s">
-        <v>1</v>
-      </c>
-      <c r="D141" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO opacheco ;</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>140</v>
-      </c>
-      <c r="B142" t="s">
-        <v>128</v>
-      </c>
-      <c r="C142" t="s">
-        <v>1</v>
-      </c>
-      <c r="D142" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO fmedeiros ;</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>140</v>
-      </c>
-      <c r="B143" t="s">
-        <v>130</v>
-      </c>
-      <c r="C143" t="s">
-        <v>1</v>
-      </c>
-      <c r="D143" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO sbhering ;</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>140</v>
-      </c>
-      <c r="B144" t="s">
-        <v>131</v>
-      </c>
-      <c r="C144" t="s">
-        <v>1</v>
-      </c>
-      <c r="D144" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO vandrade ;</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>140</v>
-      </c>
-      <c r="B145" t="s">
-        <v>129</v>
-      </c>
-      <c r="C145" t="s">
-        <v>1</v>
-      </c>
-      <c r="D145" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO dfajardo ;</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>140</v>
-      </c>
-      <c r="B146" t="s">
-        <v>132</v>
-      </c>
-      <c r="C146" t="s">
-        <v>1</v>
-      </c>
-      <c r="D146" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO jmiguel ;</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>140</v>
-      </c>
-      <c r="B147" t="s">
-        <v>133</v>
-      </c>
-      <c r="C147" t="s">
-        <v>1</v>
-      </c>
-      <c r="D147" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO coliveira ;</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>140</v>
-      </c>
-      <c r="B148" t="s">
-        <v>134</v>
-      </c>
-      <c r="C148" t="s">
-        <v>1</v>
-      </c>
-      <c r="D148" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO pferreira ;</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>140</v>
-      </c>
-      <c r="B149" t="s">
-        <v>135</v>
-      </c>
-      <c r="C149" t="s">
-        <v>1</v>
-      </c>
-      <c r="D149" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO amorais ;</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>140</v>
-      </c>
-      <c r="B150" t="s">
-        <v>136</v>
-      </c>
-      <c r="C150" t="s">
-        <v>1</v>
-      </c>
-      <c r="D150" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO poliveira ;</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>140</v>
-      </c>
-      <c r="B151" t="s">
-        <v>137</v>
-      </c>
-      <c r="C151" t="s">
-        <v>1</v>
-      </c>
-      <c r="D151" t="str">
-        <f t="shared" si="2"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status TO farmacia ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_usua_acesso to lrezende ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Grant e verificação do relatorio/impressao_relatorioportipo.php
</commit_message>
<xml_diff>
--- a/script_base_dados/grants.xlsx
+++ b/script_base_dados/grants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\integracao\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A4502B-741D-4C57-BBE5-EB87A615B1BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FC269D-A125-4D84-BBB4-4F0EE1335306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -496,7 +496,7 @@
     <t>GRANT ALL ON SEQUENCE integracao.sq_usua_acesso to</t>
   </si>
   <si>
-    <t>lrezende</t>
+    <t>wlima</t>
   </si>
 </sst>
 </file>
@@ -3753,7 +3753,7 @@
       </c>
       <c r="D59" t="str">
         <f>A59&amp;" "&amp;B59&amp;" "&amp;C59</f>
-        <v>CREATE USER  lrezende PASSWORD '1234';</v>
+        <v>CREATE USER  wlima PASSWORD '1234';</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3768,7 +3768,7 @@
       </c>
       <c r="D60" t="str">
         <f t="shared" ref="D60:D112" si="0">A60&amp;" "&amp;B60&amp;" "&amp;C60</f>
-        <v>GRANT CONNECT ON DATABASE vila_verde TO  lrezende ;</v>
+        <v>GRANT CONNECT ON DATABASE vila_verde TO  wlima ;</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3783,7 +3783,7 @@
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT USAGE ON SCHEMA integracao TO  lrezende ;</v>
+        <v>GRANT USAGE ON SCHEMA integracao TO  wlima ;</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3798,7 +3798,7 @@
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  lrezende ;</v>
+        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  wlima ;</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  lrezende ;</v>
+        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  wlima ;</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3828,7 +3828,7 @@
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO lrezende ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO wlima ;</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3843,7 +3843,7 @@
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  lrezende ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  wlima ;</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="D66" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  lrezende ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  wlima ;</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3873,7 +3873,7 @@
       </c>
       <c r="D67" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  lrezende ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  wlima ;</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3888,7 +3888,7 @@
       </c>
       <c r="D68" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  lrezende ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  wlima ;</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3903,7 +3903,7 @@
       </c>
       <c r="D69" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  lrezende ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  wlima ;</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3918,7 +3918,7 @@
       </c>
       <c r="D70" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  lrezende ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  wlima ;</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3933,7 +3933,7 @@
       </c>
       <c r="D71" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  lrezende ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  wlima ;</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3948,7 +3948,7 @@
       </c>
       <c r="D72" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  lrezende ;</v>
+        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  wlima ;</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3963,7 +3963,7 @@
       </c>
       <c r="D73" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to lrezende ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to wlima ;</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3978,7 +3978,7 @@
       </c>
       <c r="D74" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to lrezende ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to wlima ;</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3993,7 +3993,7 @@
       </c>
       <c r="D75" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to lrezende ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to wlima ;</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -4008,7 +4008,7 @@
       </c>
       <c r="D76" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to lrezende ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to wlima ;</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -4023,7 +4023,7 @@
       </c>
       <c r="D77" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to lrezende ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to wlima ;</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -4038,7 +4038,7 @@
       </c>
       <c r="D78" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to lrezende ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to wlima ;</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -4053,7 +4053,7 @@
       </c>
       <c r="D79" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to lrezende ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to wlima ;</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4068,7 +4068,7 @@
       </c>
       <c r="D80" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to lrezende ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to wlima ;</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -4083,7 +4083,7 @@
       </c>
       <c r="D81" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to lrezende ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to wlima ;</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4098,7 +4098,7 @@
       </c>
       <c r="D82" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO lrezende ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO wlima ;</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="D83" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO lrezende ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO wlima ;</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -4128,7 +4128,7 @@
       </c>
       <c r="D84" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  lrezende ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  wlima ;</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -4143,7 +4143,7 @@
       </c>
       <c r="D85" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO lrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO wlima ;</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4158,7 +4158,7 @@
       </c>
       <c r="D86" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO lrezende ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO wlima ;</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4173,7 +4173,7 @@
       </c>
       <c r="D87" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO lrezende ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO wlima ;</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="D88" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO lrezende ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO wlima ;</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4203,7 +4203,7 @@
       </c>
       <c r="D89" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO lrezende ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO wlima ;</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -4218,7 +4218,7 @@
       </c>
       <c r="D90" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  lrezende ;</v>
+        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  wlima ;</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4233,7 +4233,7 @@
       </c>
       <c r="D91" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  lrezende ;</v>
+        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  wlima ;</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4248,7 +4248,7 @@
       </c>
       <c r="D92" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_leito TO  lrezende ;</v>
+        <v>GRANT SELECT on integracao.tb_leito TO  wlima ;</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -4263,7 +4263,7 @@
       </c>
       <c r="D93" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  lrezende ;</v>
+        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  wlima ;</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4278,7 +4278,7 @@
       </c>
       <c r="D94" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_crtr_intnc TO  lrezende ;</v>
+        <v>GRANT SELECT on integracao.tb_crtr_intnc TO  wlima ;</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -4293,7 +4293,7 @@
       </c>
       <c r="D95" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_dieta TO  lrezende ;</v>
+        <v>GRANT SELECT on integracao.tb_dieta TO  wlima ;</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4308,7 +4308,7 @@
       </c>
       <c r="D96" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  lrezende ;</v>
+        <v>GRANT SELECT on integracao.tb_const TO  wlima ;</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4323,7 +4323,7 @@
       </c>
       <c r="D97" t="str">
         <f t="shared" ref="D97" si="1">A97&amp;" "&amp;B97&amp;" "&amp;C97</f>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  lrezende ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  wlima ;</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="D98" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_acesso_transac_integracao to lrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_acesso_transac_integracao to wlima ;</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4353,7 +4353,7 @@
       </c>
       <c r="D99" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_equip_hosptr to lrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_equip_hosptr to wlima ;</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4368,7 +4368,7 @@
       </c>
       <c r="D100" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_acesso to  lrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_acesso to  wlima ;</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4383,7 +4383,7 @@
       </c>
       <c r="D101" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_acesso to  lrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_acesso to  wlima ;</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4398,7 +4398,7 @@
       </c>
       <c r="D102" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_menu_sist_integracao to  lrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_menu_sist_integracao to  wlima ;</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="D103" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_transac_acesso to  lrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_transac_acesso to  wlima ;</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4428,7 +4428,7 @@
       </c>
       <c r="D104" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grvd_risco_pcnt to  lrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grvd_risco_pcnt to  wlima ;</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4443,7 +4443,7 @@
       </c>
       <c r="D105" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status to  lrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status to  wlima ;</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4458,7 +4458,7 @@
       </c>
       <c r="D106" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso to  lrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso to  wlima ;</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4473,7 +4473,7 @@
       </c>
       <c r="D107" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_menu_sist_integracao to  lrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_menu_sist_integracao to  wlima ;</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4488,7 +4488,7 @@
       </c>
       <c r="D108" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_mtvo_alta to  lrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_mtvo_alta to  wlima ;</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4503,7 +4503,7 @@
       </c>
       <c r="D109" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_orig_dmnd_plnj_leito to  lrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_orig_dmnd_plnj_leito to  wlima ;</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4518,7 +4518,7 @@
       </c>
       <c r="D110" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_plnj_pcnt_leito to  lrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_plnj_pcnt_leito to  wlima ;</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4533,7 +4533,7 @@
       </c>
       <c r="D111" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_status_leito to  lrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_status_leito to  wlima ;</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4548,7 +4548,7 @@
       </c>
       <c r="D112" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_usua_acesso to lrezende ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_usua_acesso to wlima ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alterações para acresentar funcionalidades do planejamento de demanda (controle de fila)
</commit_message>
<xml_diff>
--- a/script_base_dados/grants.xlsx
+++ b/script_base_dados/grants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\integracao\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FC269D-A125-4D84-BBB4-4F0EE1335306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C44536C-8A04-4FAA-910C-C3CD27E507F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="160">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -497,6 +497,24 @@
   </si>
   <si>
     <t>wlima</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_cnvo TO</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_grvd_risco_pcnt TO</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_moskit_cnto TO</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_orig_dmnd_plnj_leito TO</t>
+  </si>
+  <si>
+    <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_plnj_pcnt_leito TO</t>
+  </si>
+  <si>
+    <t>evaldo</t>
   </si>
 </sst>
 </file>
@@ -3342,11 +3360,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59:D112"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3761,14 +3777,14 @@
         <v>88</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C60" t="s">
         <v>1</v>
       </c>
       <c r="D60" t="str">
-        <f t="shared" ref="D60:D112" si="0">A60&amp;" "&amp;B60&amp;" "&amp;C60</f>
-        <v>GRANT CONNECT ON DATABASE vila_verde TO  wlima ;</v>
+        <f t="shared" ref="D60:D117" si="0">A60&amp;" "&amp;B60&amp;" "&amp;C60</f>
+        <v>GRANT CONNECT ON DATABASE vila_verde TO  evaldo ;</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3776,14 +3792,14 @@
         <v>66</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C61" t="s">
         <v>1</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT USAGE ON SCHEMA integracao TO  wlima ;</v>
+        <v>GRANT USAGE ON SCHEMA integracao TO  evaldo ;</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3791,14 +3807,14 @@
         <v>67</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C62" t="s">
         <v>1</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  wlima ;</v>
+        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  evaldo ;</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3806,14 +3822,14 @@
         <v>68</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C63" t="s">
         <v>1</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  wlima ;</v>
+        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  evaldo ;</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3821,14 +3837,14 @@
         <v>69</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C64" t="s">
         <v>1</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO wlima ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO evaldo ;</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3836,14 +3852,14 @@
         <v>70</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C65" t="s">
         <v>1</v>
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  wlima ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  evaldo ;</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3851,14 +3867,14 @@
         <v>71</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C66" t="s">
         <v>1</v>
       </c>
       <c r="D66" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  wlima ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  evaldo ;</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3866,14 +3882,14 @@
         <v>72</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C67" t="s">
         <v>1</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  wlima ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  evaldo ;</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3881,14 +3897,14 @@
         <v>73</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C68" t="s">
         <v>1</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  wlima ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  evaldo ;</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3896,14 +3912,14 @@
         <v>74</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C69" t="s">
         <v>1</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  wlima ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  evaldo ;</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3911,14 +3927,14 @@
         <v>75</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C70" t="s">
         <v>1</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  wlima ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  evaldo ;</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3926,14 +3942,14 @@
         <v>76</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C71" t="s">
         <v>1</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  wlima ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  evaldo ;</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3941,14 +3957,14 @@
         <v>77</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C72" t="s">
         <v>1</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  wlima ;</v>
+        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  evaldo ;</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3956,14 +3972,14 @@
         <v>27</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C73" t="s">
         <v>1</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to wlima ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to evaldo ;</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3971,14 +3987,14 @@
         <v>25</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C74" t="s">
         <v>1</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to wlima ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to evaldo ;</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3986,14 +4002,14 @@
         <v>26</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C75" t="s">
         <v>1</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to wlima ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to evaldo ;</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -4001,14 +4017,14 @@
         <v>19</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C76" t="s">
         <v>1</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to wlima ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to evaldo ;</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -4016,14 +4032,14 @@
         <v>20</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to wlima ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to evaldo ;</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -4031,14 +4047,14 @@
         <v>21</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C78" t="s">
         <v>1</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to wlima ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to evaldo ;</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -4046,14 +4062,14 @@
         <v>22</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C79" t="s">
         <v>1</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to wlima ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to evaldo ;</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4061,14 +4077,14 @@
         <v>23</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C80" t="s">
         <v>1</v>
       </c>
       <c r="D80" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to wlima ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to evaldo ;</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -4076,14 +4092,14 @@
         <v>24</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C81" t="s">
         <v>1</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to wlima ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to evaldo ;</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4091,14 +4107,14 @@
         <v>0</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C82" t="s">
         <v>1</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO wlima ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO evaldo ;</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -4106,14 +4122,14 @@
         <v>2</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C83" t="s">
         <v>1</v>
       </c>
       <c r="D83" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO wlima ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO evaldo ;</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -4121,14 +4137,14 @@
         <v>3</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C84" t="s">
         <v>1</v>
       </c>
       <c r="D84" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  wlima ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  evaldo ;</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -4136,14 +4152,14 @@
         <v>4</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C85" t="s">
         <v>1</v>
       </c>
       <c r="D85" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO wlima ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO evaldo ;</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4151,14 +4167,14 @@
         <v>5</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C86" t="s">
         <v>1</v>
       </c>
       <c r="D86" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO wlima ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO evaldo ;</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4166,14 +4182,14 @@
         <v>6</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C87" t="s">
         <v>1</v>
       </c>
       <c r="D87" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO wlima ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO evaldo ;</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -4181,14 +4197,14 @@
         <v>7</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C88" t="s">
         <v>1</v>
       </c>
       <c r="D88" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO wlima ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO evaldo ;</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4196,14 +4212,14 @@
         <v>8</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C89" t="s">
         <v>1</v>
       </c>
       <c r="D89" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO wlima ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO evaldo ;</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -4211,14 +4227,14 @@
         <v>86</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C90" t="s">
         <v>1</v>
       </c>
       <c r="D90" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  wlima ;</v>
+        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  evaldo ;</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4226,14 +4242,14 @@
         <v>87</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C91" t="s">
         <v>1</v>
       </c>
       <c r="D91" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  wlima ;</v>
+        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  evaldo ;</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4241,14 +4257,14 @@
         <v>84</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C92" t="s">
         <v>1</v>
       </c>
       <c r="D92" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_leito TO  wlima ;</v>
+        <v>GRANT SELECT on integracao.tb_leito TO  evaldo ;</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -4256,14 +4272,14 @@
         <v>85</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C93" t="s">
         <v>1</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  wlima ;</v>
+        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  evaldo ;</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4271,14 +4287,14 @@
         <v>111</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C94" t="s">
         <v>1</v>
       </c>
       <c r="D94" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_crtr_intnc TO  wlima ;</v>
+        <v>GRANT SELECT on integracao.tb_crtr_intnc TO  evaldo ;</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -4286,14 +4302,14 @@
         <v>112</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C95" t="s">
         <v>1</v>
       </c>
       <c r="D95" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_dieta TO  wlima ;</v>
+        <v>GRANT SELECT on integracao.tb_dieta TO  evaldo ;</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4301,14 +4317,14 @@
         <v>113</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C96" t="s">
         <v>1</v>
       </c>
       <c r="D96" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  wlima ;</v>
+        <v>GRANT SELECT on integracao.tb_const TO  evaldo ;</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4316,14 +4332,14 @@
         <v>137</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C97" t="s">
         <v>1</v>
       </c>
       <c r="D97" t="str">
         <f t="shared" ref="D97" si="1">A97&amp;" "&amp;B97&amp;" "&amp;C97</f>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  wlima ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  evaldo ;</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4331,14 +4347,14 @@
         <v>138</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C98" t="s">
         <v>1</v>
       </c>
       <c r="D98" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_acesso_transac_integracao to wlima ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_acesso_transac_integracao to evaldo ;</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4346,14 +4362,14 @@
         <v>139</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C99" t="s">
         <v>1</v>
       </c>
       <c r="D99" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_equip_hosptr to wlima ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_equip_hosptr to evaldo ;</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4361,14 +4377,14 @@
         <v>140</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C100" t="s">
         <v>1</v>
       </c>
       <c r="D100" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_acesso to  wlima ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_acesso to  evaldo ;</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4376,14 +4392,14 @@
         <v>141</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C101" t="s">
         <v>1</v>
       </c>
       <c r="D101" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_acesso to  wlima ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_acesso to  evaldo ;</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4391,14 +4407,14 @@
         <v>142</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C102" t="s">
         <v>1</v>
       </c>
       <c r="D102" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_menu_sist_integracao to  wlima ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_menu_sist_integracao to  evaldo ;</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4406,14 +4422,14 @@
         <v>143</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C103" t="s">
         <v>1</v>
       </c>
       <c r="D103" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_transac_acesso to  wlima ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_transac_acesso to  evaldo ;</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4421,14 +4437,14 @@
         <v>144</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C104" t="s">
         <v>1</v>
       </c>
       <c r="D104" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grvd_risco_pcnt to  wlima ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grvd_risco_pcnt to  evaldo ;</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4436,14 +4452,14 @@
         <v>145</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C105" t="s">
         <v>1</v>
       </c>
       <c r="D105" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status to  wlima ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status to  evaldo ;</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4451,14 +4467,14 @@
         <v>146</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C106" t="s">
         <v>1</v>
       </c>
       <c r="D106" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso to  wlima ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso to  evaldo ;</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4466,14 +4482,14 @@
         <v>147</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C107" t="s">
         <v>1</v>
       </c>
       <c r="D107" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_menu_sist_integracao to  wlima ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_menu_sist_integracao to  evaldo ;</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4481,14 +4497,14 @@
         <v>148</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C108" t="s">
         <v>1</v>
       </c>
       <c r="D108" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_mtvo_alta to  wlima ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_mtvo_alta to  evaldo ;</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4496,14 +4512,14 @@
         <v>149</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C109" t="s">
         <v>1</v>
       </c>
       <c r="D109" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_orig_dmnd_plnj_leito to  wlima ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_orig_dmnd_plnj_leito to  evaldo ;</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4511,14 +4527,14 @@
         <v>150</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C110" t="s">
         <v>1</v>
       </c>
       <c r="D110" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_plnj_pcnt_leito to  wlima ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_plnj_pcnt_leito to  evaldo ;</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4526,14 +4542,14 @@
         <v>151</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C111" t="s">
         <v>1</v>
       </c>
       <c r="D111" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_status_leito to  wlima ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_status_leito to  evaldo ;</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4541,14 +4557,89 @@
         <v>152</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C112" t="s">
         <v>1</v>
       </c>
       <c r="D112" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_usua_acesso to wlima ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_usua_acesso to evaldo ;</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>154</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C113" t="s">
+        <v>1</v>
+      </c>
+      <c r="D113" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_cnvo TO evaldo ;</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>155</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C114" t="s">
+        <v>1</v>
+      </c>
+      <c r="D114" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_grvd_risco_pcnt TO evaldo ;</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>156</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C115" t="s">
+        <v>1</v>
+      </c>
+      <c r="D115" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_moskit_cnto TO evaldo ;</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>157</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C116" t="s">
+        <v>1</v>
+      </c>
+      <c r="D116" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_orig_dmnd_plnj_leito TO evaldo ;</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>158</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C117" t="s">
+        <v>1</v>
+      </c>
+      <c r="D117" t="str">
+        <f t="shared" si="0"/>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_plnj_pcnt_leito TO evaldo ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização do planejamento da demanda
</commit_message>
<xml_diff>
--- a/script_base_dados/grants.xlsx
+++ b/script_base_dados/grants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\integracao\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C44536C-8A04-4FAA-910C-C3CD27E507F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE82795-C31E-403E-946A-36049024B8B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="159">
   <si>
     <t>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO</t>
   </si>
@@ -496,9 +496,6 @@
     <t>GRANT ALL ON SEQUENCE integracao.sq_usua_acesso to</t>
   </si>
   <si>
-    <t>wlima</t>
-  </si>
-  <si>
     <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_cnvo TO</t>
   </si>
   <si>
@@ -514,7 +511,7 @@
     <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_plnj_pcnt_leito TO</t>
   </si>
   <si>
-    <t>evaldo</t>
+    <t>yago</t>
   </si>
 </sst>
 </file>
@@ -3362,7 +3359,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
   <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D117" sqref="D59:D117"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3762,14 +3761,14 @@
         <v>78</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C59" t="s">
         <v>79</v>
       </c>
       <c r="D59" t="str">
         <f>A59&amp;" "&amp;B59&amp;" "&amp;C59</f>
-        <v>CREATE USER  wlima PASSWORD '1234';</v>
+        <v>CREATE USER  yago PASSWORD '1234';</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3777,14 +3776,14 @@
         <v>88</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C60" t="s">
         <v>1</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" ref="D60:D117" si="0">A60&amp;" "&amp;B60&amp;" "&amp;C60</f>
-        <v>GRANT CONNECT ON DATABASE vila_verde TO  evaldo ;</v>
+        <v>GRANT CONNECT ON DATABASE vila_verde TO  yago ;</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3792,14 +3791,14 @@
         <v>66</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C61" t="s">
         <v>1</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT USAGE ON SCHEMA integracao TO  evaldo ;</v>
+        <v>GRANT USAGE ON SCHEMA integracao TO  yago ;</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3807,14 +3806,14 @@
         <v>67</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C62" t="s">
         <v>1</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  evaldo ;</v>
+        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  yago ;</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3822,14 +3821,14 @@
         <v>68</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C63" t="s">
         <v>1</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  evaldo ;</v>
+        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  yago ;</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3837,14 +3836,14 @@
         <v>69</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C64" t="s">
         <v>1</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO evaldo ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO yago ;</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3852,14 +3851,14 @@
         <v>70</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C65" t="s">
         <v>1</v>
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  evaldo ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  yago ;</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3867,14 +3866,14 @@
         <v>71</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C66" t="s">
         <v>1</v>
       </c>
       <c r="D66" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  evaldo ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  yago ;</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3882,14 +3881,14 @@
         <v>72</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C67" t="s">
         <v>1</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  evaldo ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  yago ;</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3897,14 +3896,14 @@
         <v>73</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C68" t="s">
         <v>1</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  evaldo ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  yago ;</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3912,14 +3911,14 @@
         <v>74</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C69" t="s">
         <v>1</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  evaldo ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  yago ;</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3927,14 +3926,14 @@
         <v>75</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C70" t="s">
         <v>1</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  evaldo ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  yago ;</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3942,14 +3941,14 @@
         <v>76</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C71" t="s">
         <v>1</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  evaldo ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  yago ;</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3957,14 +3956,14 @@
         <v>77</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C72" t="s">
         <v>1</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  evaldo ;</v>
+        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  yago ;</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3972,14 +3971,14 @@
         <v>27</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C73" t="s">
         <v>1</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to yago ;</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3987,14 +3986,14 @@
         <v>25</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C74" t="s">
         <v>1</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to yago ;</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -4002,14 +4001,14 @@
         <v>26</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C75" t="s">
         <v>1</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to yago ;</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -4017,14 +4016,14 @@
         <v>19</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C76" t="s">
         <v>1</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to yago ;</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -4032,14 +4031,14 @@
         <v>20</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to yago ;</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -4047,14 +4046,14 @@
         <v>21</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C78" t="s">
         <v>1</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to yago ;</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -4062,14 +4061,14 @@
         <v>22</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C79" t="s">
         <v>1</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to yago ;</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4077,14 +4076,14 @@
         <v>23</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C80" t="s">
         <v>1</v>
       </c>
       <c r="D80" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to yago ;</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -4092,14 +4091,14 @@
         <v>24</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C81" t="s">
         <v>1</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to yago ;</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4107,14 +4106,14 @@
         <v>0</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C82" t="s">
         <v>1</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO evaldo ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO yago ;</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -4122,14 +4121,14 @@
         <v>2</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C83" t="s">
         <v>1</v>
       </c>
       <c r="D83" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO evaldo ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO yago ;</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -4137,14 +4136,14 @@
         <v>3</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C84" t="s">
         <v>1</v>
       </c>
       <c r="D84" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  evaldo ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  yago ;</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -4152,14 +4151,14 @@
         <v>4</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C85" t="s">
         <v>1</v>
       </c>
       <c r="D85" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO yago ;</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4167,14 +4166,14 @@
         <v>5</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C86" t="s">
         <v>1</v>
       </c>
       <c r="D86" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO yago ;</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4182,14 +4181,14 @@
         <v>6</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C87" t="s">
         <v>1</v>
       </c>
       <c r="D87" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO yago ;</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -4197,14 +4196,14 @@
         <v>7</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C88" t="s">
         <v>1</v>
       </c>
       <c r="D88" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO yago ;</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4212,14 +4211,14 @@
         <v>8</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C89" t="s">
         <v>1</v>
       </c>
       <c r="D89" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO yago ;</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -4227,14 +4226,14 @@
         <v>86</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C90" t="s">
         <v>1</v>
       </c>
       <c r="D90" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  evaldo ;</v>
+        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  yago ;</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4242,14 +4241,14 @@
         <v>87</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C91" t="s">
         <v>1</v>
       </c>
       <c r="D91" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  evaldo ;</v>
+        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  yago ;</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4257,14 +4256,14 @@
         <v>84</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C92" t="s">
         <v>1</v>
       </c>
       <c r="D92" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_leito TO  evaldo ;</v>
+        <v>GRANT SELECT on integracao.tb_leito TO  yago ;</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -4272,14 +4271,14 @@
         <v>85</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C93" t="s">
         <v>1</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  evaldo ;</v>
+        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  yago ;</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4287,14 +4286,14 @@
         <v>111</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C94" t="s">
         <v>1</v>
       </c>
       <c r="D94" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_crtr_intnc TO  evaldo ;</v>
+        <v>GRANT SELECT on integracao.tb_crtr_intnc TO  yago ;</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -4302,14 +4301,14 @@
         <v>112</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C95" t="s">
         <v>1</v>
       </c>
       <c r="D95" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_dieta TO  evaldo ;</v>
+        <v>GRANT SELECT on integracao.tb_dieta TO  yago ;</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4317,14 +4316,14 @@
         <v>113</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C96" t="s">
         <v>1</v>
       </c>
       <c r="D96" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  evaldo ;</v>
+        <v>GRANT SELECT on integracao.tb_const TO  yago ;</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4332,14 +4331,14 @@
         <v>137</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C97" t="s">
         <v>1</v>
       </c>
       <c r="D97" t="str">
         <f t="shared" ref="D97" si="1">A97&amp;" "&amp;B97&amp;" "&amp;C97</f>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  evaldo ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  yago ;</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4347,14 +4346,14 @@
         <v>138</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C98" t="s">
         <v>1</v>
       </c>
       <c r="D98" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_acesso_transac_integracao to evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_acesso_transac_integracao to yago ;</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4362,14 +4361,14 @@
         <v>139</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C99" t="s">
         <v>1</v>
       </c>
       <c r="D99" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_equip_hosptr to evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_equip_hosptr to yago ;</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4377,14 +4376,14 @@
         <v>140</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C100" t="s">
         <v>1</v>
       </c>
       <c r="D100" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_acesso to  evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_acesso to  yago ;</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4392,14 +4391,14 @@
         <v>141</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C101" t="s">
         <v>1</v>
       </c>
       <c r="D101" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_acesso to  evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_acesso to  yago ;</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4407,14 +4406,14 @@
         <v>142</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C102" t="s">
         <v>1</v>
       </c>
       <c r="D102" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_menu_sist_integracao to  evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_menu_sist_integracao to  yago ;</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4422,14 +4421,14 @@
         <v>143</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C103" t="s">
         <v>1</v>
       </c>
       <c r="D103" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_transac_acesso to  evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_transac_acesso to  yago ;</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4437,14 +4436,14 @@
         <v>144</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C104" t="s">
         <v>1</v>
       </c>
       <c r="D104" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grvd_risco_pcnt to  evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grvd_risco_pcnt to  yago ;</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4452,14 +4451,14 @@
         <v>145</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C105" t="s">
         <v>1</v>
       </c>
       <c r="D105" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status to  evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status to  yago ;</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4467,14 +4466,14 @@
         <v>146</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C106" t="s">
         <v>1</v>
       </c>
       <c r="D106" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso to  evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso to  yago ;</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4482,14 +4481,14 @@
         <v>147</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C107" t="s">
         <v>1</v>
       </c>
       <c r="D107" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_menu_sist_integracao to  evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_menu_sist_integracao to  yago ;</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4497,14 +4496,14 @@
         <v>148</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C108" t="s">
         <v>1</v>
       </c>
       <c r="D108" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_mtvo_alta to  evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_mtvo_alta to  yago ;</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4512,14 +4511,14 @@
         <v>149</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C109" t="s">
         <v>1</v>
       </c>
       <c r="D109" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_orig_dmnd_plnj_leito to  evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_orig_dmnd_plnj_leito to  yago ;</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4527,14 +4526,14 @@
         <v>150</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C110" t="s">
         <v>1</v>
       </c>
       <c r="D110" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_plnj_pcnt_leito to  evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_plnj_pcnt_leito to  yago ;</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4542,14 +4541,14 @@
         <v>151</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C111" t="s">
         <v>1</v>
       </c>
       <c r="D111" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_status_leito to  evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_status_leito to  yago ;</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4557,89 +4556,89 @@
         <v>152</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C112" t="s">
         <v>1</v>
       </c>
       <c r="D112" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_usua_acesso to evaldo ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_usua_acesso to yago ;</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C113" t="s">
         <v>1</v>
       </c>
       <c r="D113" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_cnvo TO evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_cnvo TO yago ;</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C114" t="s">
         <v>1</v>
       </c>
       <c r="D114" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_grvd_risco_pcnt TO evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_grvd_risco_pcnt TO yago ;</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C115" t="s">
         <v>1</v>
       </c>
       <c r="D115" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_moskit_cnto TO evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_moskit_cnto TO yago ;</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C116" t="s">
         <v>1</v>
       </c>
       <c r="D116" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_orig_dmnd_plnj_leito TO evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_orig_dmnd_plnj_leito TO yago ;</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C117" t="s">
         <v>1</v>
       </c>
       <c r="D117" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_plnj_pcnt_leito TO evaldo ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_plnj_pcnt_leito TO yago ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Grupo de CID e CID
</commit_message>
<xml_diff>
--- a/script_base_dados/grants.xlsx
+++ b/script_base_dados/grants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\integracao\script_base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D0737B-8E03-4155-A398-3FDF369E2E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEF1DC9-DCD0-4B16-9676-42012D3BA891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7CE13645-C895-4B7C-AE75-E38469D152AE}"/>
   </bookViews>
@@ -511,7 +511,7 @@
     <t>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_plnj_pcnt_leito TO</t>
   </si>
   <si>
-    <t>goliveira</t>
+    <t>dmansur</t>
   </si>
 </sst>
 </file>
@@ -3359,8 +3359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5A992-25FF-475C-9CF2-7DC64A66C30C}">
   <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59:D125"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59:D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3768,7 +3768,7 @@
       </c>
       <c r="D59" t="str">
         <f>A59&amp;" "&amp;B59&amp;" "&amp;C59</f>
-        <v>CREATE USER  goliveira PASSWORD '1234';</v>
+        <v>CREATE USER  dmansur PASSWORD '1234';</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3783,7 +3783,7 @@
       </c>
       <c r="D60" t="str">
         <f t="shared" ref="D60:D117" si="0">A60&amp;" "&amp;B60&amp;" "&amp;C60</f>
-        <v>GRANT CONNECT ON DATABASE vila_verde TO  goliveira ;</v>
+        <v>GRANT CONNECT ON DATABASE vila_verde TO  dmansur ;</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3798,7 +3798,7 @@
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT USAGE ON SCHEMA integracao TO  goliveira ;</v>
+        <v>GRANT USAGE ON SCHEMA integracao TO  dmansur ;</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  goliveira ;</v>
+        <v>GRANT SELECT ON ALL TABLES IN SCHEMA integracao TO  dmansur ;</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3828,7 +3828,7 @@
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  goliveira ;</v>
+        <v>GRANT SELECT, UPDATE, DELETE, INSERT ON ALL TABLES IN SCHEMA integracao TO  dmansur ;</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3843,7 +3843,7 @@
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO goliveira ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao TO dmansur ;</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  goliveira ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_integracao_usua TO  dmansur ;</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3873,7 +3873,7 @@
       </c>
       <c r="D66" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  goliveira ;</v>
+        <v>GRANT SELECT on integracao.vw_menu_princ_usua TO  dmansur ;</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3888,7 +3888,7 @@
       </c>
       <c r="D67" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  goliveira ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_acesso TO  dmansur ;</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3903,7 +3903,7 @@
       </c>
       <c r="D68" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  goliveira ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_acesso TO  dmansur ;</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3918,7 +3918,7 @@
       </c>
       <c r="D69" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  goliveira ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_grupo_usua_menu_sist_integracao TO  dmansur ;</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3933,7 +3933,7 @@
       </c>
       <c r="D70" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  goliveira ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_menu_sist_integracao TO  dmansur ;</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3948,7 +3948,7 @@
       </c>
       <c r="D71" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  goliveira ;</v>
+        <v>GRANT SELECT, UPDATE, INSERT, DELETE ON integracao.tb_c_usua_acesso TO  dmansur ;</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3963,7 +3963,7 @@
       </c>
       <c r="D72" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  goliveira ;</v>
+        <v>GRANT DELETE, UPDATE, INSERT, SELECT ON integracao.tb_c_log_acesso TO  dmansur ;</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3978,7 +3978,7 @@
       </c>
       <c r="D73" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_cid to dmansur ;</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3993,7 +3993,7 @@
       </c>
       <c r="D74" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_equip_hosptr to dmansur ;</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -4008,7 +4008,7 @@
       </c>
       <c r="D75" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_status_leito to dmansur ;</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -4023,7 +4023,7 @@
       </c>
       <c r="D76" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_acesso to dmansur ;</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -4038,7 +4038,7 @@
       </c>
       <c r="D77" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_acesso to dmansur ;</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -4053,7 +4053,7 @@
       </c>
       <c r="D78" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_log_acesso to dmansur ;</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -4068,7 +4068,7 @@
       </c>
       <c r="D79" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_grupo_usua_menu_sist_integracao to dmansur ;</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4083,7 +4083,7 @@
       </c>
       <c r="D80" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_menu_sist_integracao to dmansur ;</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -4098,7 +4098,7 @@
       </c>
       <c r="D81" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_c_usua_acesso to dmansur ;</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="D82" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO goliveira ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao TO dmansur ;</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -4128,7 +4128,7 @@
       </c>
       <c r="D83" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO goliveira ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_integracao_usua TO dmansur ;</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -4143,7 +4143,7 @@
       </c>
       <c r="D84" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  goliveira ;</v>
+        <v>GRANT SELECT ON TABLE integracao.vw_menu_princ_usua TO  dmansur ;</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -4158,7 +4158,7 @@
       </c>
       <c r="D85" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO goliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso TO dmansur ;</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4173,7 +4173,7 @@
       </c>
       <c r="D86" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_smart TO dmansur ;</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4188,7 +4188,7 @@
       </c>
       <c r="D87" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_f_hstr_ocpa_leito_status TO dmansur ;</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -4203,7 +4203,7 @@
       </c>
       <c r="D88" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito_temp TO dmansur ;</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4218,7 +4218,7 @@
       </c>
       <c r="D89" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_ctrl_leito TO dmansur ;</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -4233,7 +4233,7 @@
       </c>
       <c r="D90" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  goliveira ;</v>
+        <v>GRANT SELECT on integracao.tb_mtvo_alta TO  dmansur ;</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4248,7 +4248,7 @@
       </c>
       <c r="D91" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  goliveira ;</v>
+        <v>GRANT SELECT, update, insert, delete on integracao.tb_bmh_online TO  dmansur ;</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4263,7 +4263,7 @@
       </c>
       <c r="D92" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_leito TO  goliveira ;</v>
+        <v>GRANT SELECT on integracao.tb_leito TO  dmansur ;</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -4278,7 +4278,7 @@
       </c>
       <c r="D93" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  goliveira ;</v>
+        <v>GRANT SELECT on integracao.vw_ctrl_leito TO  dmansur ;</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4293,7 +4293,7 @@
       </c>
       <c r="D94" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_crtr_intnc TO  goliveira ;</v>
+        <v>GRANT SELECT on integracao.tb_crtr_intnc TO  dmansur ;</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -4308,7 +4308,7 @@
       </c>
       <c r="D95" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_dieta TO  goliveira ;</v>
+        <v>GRANT SELECT on integracao.tb_dieta TO  dmansur ;</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4323,7 +4323,7 @@
       </c>
       <c r="D96" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT on integracao.tb_const TO  goliveira ;</v>
+        <v>GRANT SELECT on integracao.tb_const TO  dmansur ;</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="D97" t="str">
         <f t="shared" ref="D97" si="1">A97&amp;" "&amp;B97&amp;" "&amp;C97</f>
-        <v>GRANT SELECT on integracao.vw_bmh_online TO  goliveira ;</v>
+        <v>GRANT SELECT on integracao.vw_bmh_online TO  dmansur ;</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4353,7 +4353,7 @@
       </c>
       <c r="D98" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_acesso_transac_integracao to goliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_acesso_transac_integracao to dmansur ;</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4368,7 +4368,7 @@
       </c>
       <c r="D99" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_equip_hosptr to goliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_equip_hosptr to dmansur ;</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4383,7 +4383,7 @@
       </c>
       <c r="D100" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_acesso to  goliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_acesso to  dmansur ;</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4398,7 +4398,7 @@
       </c>
       <c r="D101" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_acesso to  goliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_acesso to  dmansur ;</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="D102" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_menu_sist_integracao to  goliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_menu_sist_integracao to  dmansur ;</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4428,7 +4428,7 @@
       </c>
       <c r="D103" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_transac_acesso to  goliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grupo_usua_transac_acesso to  dmansur ;</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4443,7 +4443,7 @@
       </c>
       <c r="D104" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_grvd_risco_pcnt to  goliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_grvd_risco_pcnt to  dmansur ;</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4458,7 +4458,7 @@
       </c>
       <c r="D105" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status to  goliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_hstr_ocpa_leito_status to  dmansur ;</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4473,7 +4473,7 @@
       </c>
       <c r="D106" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso to  goliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_log_acesso to  dmansur ;</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4488,7 +4488,7 @@
       </c>
       <c r="D107" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_menu_sist_integracao to  goliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_menu_sist_integracao to  dmansur ;</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4503,7 +4503,7 @@
       </c>
       <c r="D108" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_mtvo_alta to  goliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_mtvo_alta to  dmansur ;</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4518,7 +4518,7 @@
       </c>
       <c r="D109" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_orig_dmnd_plnj_leito to  goliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_orig_dmnd_plnj_leito to  dmansur ;</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4533,7 +4533,7 @@
       </c>
       <c r="D110" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_plnj_pcnt_leito to  goliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_plnj_pcnt_leito to  dmansur ;</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4548,7 +4548,7 @@
       </c>
       <c r="D111" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_status_leito to  goliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_status_leito to  dmansur ;</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4563,7 +4563,7 @@
       </c>
       <c r="D112" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT ALL ON SEQUENCE integracao.sq_usua_acesso to goliveira ;</v>
+        <v>GRANT ALL ON SEQUENCE integracao.sq_usua_acesso to dmansur ;</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -4578,7 +4578,7 @@
       </c>
       <c r="D113" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_cnvo TO goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_cnvo TO dmansur ;</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -4593,7 +4593,7 @@
       </c>
       <c r="D114" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_grvd_risco_pcnt TO goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_grvd_risco_pcnt TO dmansur ;</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -4608,7 +4608,7 @@
       </c>
       <c r="D115" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_moskit_cnto TO goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_moskit_cnto TO dmansur ;</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -4623,7 +4623,7 @@
       </c>
       <c r="D116" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_orig_dmnd_plnj_leito TO goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_orig_dmnd_plnj_leito TO dmansur ;</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -4638,7 +4638,7 @@
       </c>
       <c r="D117" t="str">
         <f t="shared" si="0"/>
-        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_plnj_pcnt_leito TO goliveira ;</v>
+        <v>GRANT SELECT, INSERT, DELETE, UPDATE ON TABLE integracao.tb_plnj_pcnt_leito TO dmansur ;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>